<commit_message>
export cp a export cp int
</commit_message>
<xml_diff>
--- a/one folder to rule them all/Hlavna aplikacia/CPINT.xlsx
+++ b/one folder to rule them all/Hlavna aplikacia/CPINT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="Tento_zošit"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domko\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Praca_LM\Študenti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E63EF2-7B23-4E80-822B-96330643961E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A705B0-AC59-4807-9900-7AE6A03A3442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CP" sheetId="30" r:id="rId1"/>
@@ -24,12 +24,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="86">
   <si>
     <t>ks</t>
   </si>
@@ -109,9 +120,54 @@
     <t>Zamykací mechanizmus pre dvere nástennej skrine</t>
   </si>
   <si>
+    <t>Odhad pracovnej činnosti</t>
+  </si>
+  <si>
+    <t>Počet osôb</t>
+  </si>
+  <si>
+    <t>Hodiny</t>
+  </si>
+  <si>
+    <t>Plat €/h</t>
+  </si>
+  <si>
+    <t>Projektant</t>
+  </si>
+  <si>
+    <t>SLP technik</t>
+  </si>
+  <si>
+    <t>Stavbyvedúci</t>
+  </si>
+  <si>
+    <t>IP technik</t>
+  </si>
+  <si>
+    <t>Nákup materiál SPOLU</t>
+  </si>
+  <si>
+    <t>Marža</t>
+  </si>
+  <si>
+    <t>Práca nákup</t>
+  </si>
+  <si>
+    <t>Práca predaj SPOLU</t>
+  </si>
+  <si>
+    <t>Marža [%]</t>
+  </si>
+  <si>
+    <t>Dodávateľ</t>
+  </si>
+  <si>
     <t>Cenová ponuka</t>
   </si>
   <si>
+    <t>Predaj</t>
+  </si>
+  <si>
     <t xml:space="preserve">Záručná doba na pasívne časti systému (kabeláž, rozvádzače, konektory) je 60mesiacov. </t>
   </si>
   <si>
@@ -142,15 +198,51 @@
     <t>Prístupový a zabezpečovací systém (ACS/EZS)</t>
   </si>
   <si>
+    <t>Koeficient 
+(Prirážka materiál)</t>
+  </si>
+  <si>
+    <t>Nákup materiál</t>
+  </si>
+  <si>
+    <t>Nákupná materiál spolu</t>
+  </si>
+  <si>
+    <t>Počet výjazdov</t>
+  </si>
+  <si>
+    <t>Celková cena</t>
+  </si>
+  <si>
+    <t>1 výjazd v BA
+(Tam aj späť)</t>
+  </si>
+  <si>
+    <t>Mimo BA
+[€/km]</t>
+  </si>
+  <si>
+    <t>Zisk materiál SPOLU</t>
+  </si>
+  <si>
+    <t>Zisk materiál spolu [€]</t>
+  </si>
+  <si>
     <t>Práca:</t>
   </si>
   <si>
     <t>Materiál:</t>
   </si>
   <si>
+    <t>Zisk práca SPOLU</t>
+  </si>
+  <si>
     <t>Vypracoval:</t>
   </si>
   <si>
+    <t>Predaj materiál SPOLU</t>
+  </si>
+  <si>
     <t>Suma materiál:</t>
   </si>
   <si>
@@ -166,6 +258,9 @@
     <t>Optická prípojka hál DC1 a DC2 - Etapa 1</t>
   </si>
   <si>
+    <t>https://www.tesshop.sk/fibrain-mk-lxs6-opticky-kabel-72-vlakno-g-657a1-5-6mm-6t12f-metrojet_d5439.html</t>
+  </si>
+  <si>
     <t>m</t>
   </si>
   <si>
@@ -175,6 +270,12 @@
     <t>Optická spojka 144F, 72F, (2) držiak (6) kazeta (9) SC-simplex</t>
   </si>
   <si>
+    <t>https://www.tesshop.sk/fibrain-fobp-t1-opticka-spojka-144f-72f-2-drziak-6-kazeta-9-sc-simplex_d9197.html</t>
+  </si>
+  <si>
+    <t>https://www.tesshop.sk/fibrain-scm-c-12h-gy-opticka-kazeta-pre-12-zvarov_d6514.html</t>
+  </si>
+  <si>
     <t>Optická kazeta pre 12 zvarov</t>
   </si>
   <si>
@@ -185,6 +286,9 @@
   </si>
   <si>
     <t>Platnosť cenovej ponuky: dd.mm.rrrr</t>
+  </si>
+  <si>
+    <t>Skúška správnosti</t>
   </si>
   <si>
     <t>xxx, +421 9..., xxx@lastmile.sk</t>
@@ -203,15 +307,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="#,##0.00&quot; Sk&quot;"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ _S_k"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.00\ _S_k_-;\-* #,##0.00\ _S_k_-;_-* &quot;-&quot;??\ _S_k_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0.00\ &quot;Sk&quot;_-;\-* #,##0.00\ &quot;Sk&quot;_-;_-* &quot;-&quot;??\ &quot;Sk&quot;_-;_-@_-"/>
     <numFmt numFmtId="168" formatCode="#,##0.00\ [$€-1]"/>
+    <numFmt numFmtId="169" formatCode="#,##0.00\ [$€-2]"/>
     <numFmt numFmtId="170" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="52">
+  <fonts count="55">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -483,6 +588,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Tahoma"/>
@@ -528,6 +641,21 @@
       <charset val="238"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
       <sz val="16"/>
       <name val="Tahoma"/>
       <family val="2"/>
@@ -578,7 +706,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -673,6 +801,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFBF8F00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD966"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF548235"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF305496"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9D08E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8EA9DB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF3734B"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -705,8 +881,14 @@
         </stop>
       </gradientFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7575"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="49">
+  <borders count="60">
     <border>
       <left/>
       <right/>
@@ -881,6 +1063,19 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -911,7 +1106,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -920,6 +1115,112 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -1253,6 +1554,32 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1368,7 +1695,7 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1388,6 +1715,24 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="168" fontId="26" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="26" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="20" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="20" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="20" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="168" fontId="37" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1409,26 +1754,68 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="59" applyFont="1"/>
+    <xf numFmtId="49" fontId="46" fillId="0" borderId="0" xfId="59" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="43" fillId="24" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="43" fillId="25" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="18" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="18" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="18" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="26" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="31" fillId="18" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="31" fillId="18" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="18" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="18" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="18" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="31" fillId="18" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="31" fillId="18" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="31" fillId="18" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="31" fillId="18" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="18" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1437,19 +1824,19 @@
     <xf numFmtId="0" fontId="32" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="18" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="18" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="18" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="165" fontId="31" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -1457,311 +1844,390 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="42" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="47" fillId="18" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="18" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="43" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="50" fillId="18" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="48" fillId="18" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="51" fillId="18" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="42" fillId="18" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="43" fillId="18" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="48" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="51" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="42" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="46" fillId="20" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="43" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="49" fillId="28" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="20" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="28" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="20" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="28" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="47" fillId="20" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="50" fillId="28" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="40" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="41" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="37" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="20" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="28" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="48" fillId="20" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="51" fillId="28" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="20" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="28" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="170" fontId="28" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="42" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="43" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="41" fillId="19" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="42" fillId="27" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="41" fillId="18" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="18" borderId="42" xfId="60" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="18" borderId="43" xfId="60" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="18" borderId="44" xfId="60" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="21" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="42" fillId="18" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="18" borderId="51" xfId="60" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="18" borderId="52" xfId="60" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="18" borderId="53" xfId="60" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="29" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="42" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="18" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="18" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="18" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="30" xfId="60" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="19" xfId="60" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="31" xfId="60" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="20" xfId="60" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="43" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="18" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="18" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="18" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="39" xfId="60" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="28" xfId="60" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="40" xfId="60" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="29" xfId="60" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="44" fillId="0" borderId="45" xfId="60" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="45" fillId="0" borderId="54" xfId="60" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="18" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="18" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="18" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="18" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="21" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="21" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="21" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="21" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="18" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="18" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="18" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="29" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="29" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="29" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="29" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="37" fillId="22" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="26" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="37" fillId="30" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="37" fillId="22" borderId="40" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="30" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="18" borderId="46" xfId="60" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="18" borderId="47" xfId="60" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="18" borderId="48" xfId="60" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="43" fillId="26" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="43" fillId="26" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="26" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="26" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="18" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="43" fillId="32" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="18" borderId="57" xfId="60" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="18" borderId="58" xfId="60" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="18" borderId="59" xfId="60" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="37" fillId="0" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="0" borderId="47" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="37" fillId="0" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="168" fontId="37" fillId="0" borderId="47" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="34" xfId="59" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="59" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="35" xfId="59" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="26" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="26" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="23" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="26" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="26" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="21" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="21" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="23" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="31" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="23" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="31" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="23" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="31" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="23" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="31" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="23" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="31" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="23" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="31" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="23" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="21" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="21" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="31" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="23" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="31" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="23" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="31" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="23" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="31" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="23" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="31" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="23" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="31" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="25" xfId="59" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="59" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="26" xfId="59" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="170" fontId="26" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="61">
@@ -1827,7 +2293,48 @@
     <cellStyle name="Zvýraznenie5 2" xfId="57" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
     <cellStyle name="Zvýraznenie6 2" xfId="58" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1918,7 +2425,7 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>248</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>169678</xdr:rowOff>
+      <xdr:rowOff>169677</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2274,1297 +2781,1935 @@
   <sheetPr codeName="Hárok1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AD68"/>
+  <dimension ref="A1:AM68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="L1:T69"/>
+      <pane ySplit="12" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultRowHeight="14.6" outlineLevelRow="1"/>
   <cols>
-    <col min="2" max="2" width="8.33203125" customWidth="1"/>
-    <col min="3" max="3" width="78.5546875" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="8.3046875" customWidth="1"/>
+    <col min="3" max="3" width="78.53515625" customWidth="1"/>
+    <col min="4" max="4" width="8.3046875" customWidth="1"/>
+    <col min="5" max="5" width="8.15234375" customWidth="1"/>
+    <col min="6" max="6" width="19.15234375" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" customWidth="1"/>
-    <col min="13" max="13" width="10.109375" customWidth="1"/>
+    <col min="11" max="11" width="19.69140625" customWidth="1"/>
+    <col min="12" max="12" width="8.3828125" customWidth="1"/>
+    <col min="13" max="13" width="14.84375" customWidth="1"/>
+    <col min="14" max="14" width="15.3828125" customWidth="1"/>
+    <col min="15" max="15" width="13.53515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.53515625" customWidth="1"/>
+    <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14" customWidth="1"/>
+    <col min="19" max="19" width="11.3828125" customWidth="1"/>
+    <col min="20" max="20" width="17.69140625" customWidth="1"/>
+    <col min="21" max="21" width="13.3046875" customWidth="1"/>
+    <col min="22" max="22" width="10.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1"/>
-    <row r="2" spans="1:11" ht="18" customHeight="1" outlineLevel="1">
+    <row r="1" spans="1:20" ht="15" thickBot="1"/>
+    <row r="2" spans="1:20" ht="18" customHeight="1" outlineLevel="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="24"/>
-    </row>
-    <row r="3" spans="1:11" ht="32.25" customHeight="1" outlineLevel="1">
+      <c r="B2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="46"/>
+    </row>
+    <row r="3" spans="1:20" ht="32.25" customHeight="1" outlineLevel="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="134"/>
-      <c r="E3" s="134"/>
-      <c r="F3" s="134"/>
-      <c r="G3" s="134"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="28"/>
-    </row>
-    <row r="4" spans="1:11" ht="21.75" customHeight="1" outlineLevel="1">
+      <c r="B3" s="47"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="183"/>
+      <c r="E3" s="183"/>
+      <c r="F3" s="183"/>
+      <c r="G3" s="183"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="50"/>
+    </row>
+    <row r="4" spans="1:20" ht="21.75" customHeight="1" outlineLevel="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="134"/>
-      <c r="E4" s="134"/>
-      <c r="F4" s="134"/>
-      <c r="G4" s="134"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="28"/>
-    </row>
-    <row r="5" spans="1:11" ht="54" customHeight="1" outlineLevel="1" thickBot="1">
+      <c r="B4" s="47"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="183"/>
+      <c r="E4" s="183"/>
+      <c r="F4" s="183"/>
+      <c r="G4" s="183"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="50"/>
+    </row>
+    <row r="5" spans="1:20" ht="54" customHeight="1" outlineLevel="1" thickBot="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="31"/>
-    </row>
-    <row r="6" spans="1:11" outlineLevel="1">
+      <c r="B5" s="51"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="53"/>
+    </row>
+    <row r="6" spans="1:20" outlineLevel="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="135" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="136"/>
-      <c r="D6" s="136"/>
-      <c r="E6" s="136"/>
-      <c r="F6" s="136"/>
-      <c r="G6" s="136"/>
-      <c r="H6" s="136"/>
-      <c r="I6" s="136"/>
-      <c r="J6" s="136"/>
-      <c r="K6" s="137"/>
-    </row>
-    <row r="7" spans="1:11" outlineLevel="1">
+      <c r="B6" s="184" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="185"/>
+      <c r="D6" s="185"/>
+      <c r="E6" s="185"/>
+      <c r="F6" s="185"/>
+      <c r="G6" s="185"/>
+      <c r="H6" s="185"/>
+      <c r="I6" s="185"/>
+      <c r="J6" s="185"/>
+      <c r="K6" s="186"/>
+    </row>
+    <row r="7" spans="1:20" outlineLevel="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="138"/>
-      <c r="C7" s="139"/>
-      <c r="D7" s="139"/>
-      <c r="E7" s="139"/>
-      <c r="F7" s="139"/>
-      <c r="G7" s="139"/>
-      <c r="H7" s="139"/>
-      <c r="I7" s="139"/>
-      <c r="J7" s="139"/>
-      <c r="K7" s="140"/>
-    </row>
-    <row r="8" spans="1:11" outlineLevel="1">
+      <c r="B7" s="187"/>
+      <c r="C7" s="188"/>
+      <c r="D7" s="188"/>
+      <c r="E7" s="188"/>
+      <c r="F7" s="188"/>
+      <c r="G7" s="188"/>
+      <c r="H7" s="188"/>
+      <c r="I7" s="188"/>
+      <c r="J7" s="188"/>
+      <c r="K7" s="189"/>
+    </row>
+    <row r="8" spans="1:20" outlineLevel="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="138"/>
-      <c r="C8" s="139"/>
-      <c r="D8" s="139"/>
-      <c r="E8" s="139"/>
-      <c r="F8" s="139"/>
-      <c r="G8" s="139"/>
-      <c r="H8" s="139"/>
-      <c r="I8" s="139"/>
-      <c r="J8" s="139"/>
-      <c r="K8" s="140"/>
-    </row>
-    <row r="9" spans="1:11" ht="31.5" customHeight="1" outlineLevel="1">
+      <c r="B8" s="187"/>
+      <c r="C8" s="188"/>
+      <c r="D8" s="188"/>
+      <c r="E8" s="188"/>
+      <c r="F8" s="188"/>
+      <c r="G8" s="188"/>
+      <c r="H8" s="188"/>
+      <c r="I8" s="188"/>
+      <c r="J8" s="188"/>
+      <c r="K8" s="189"/>
+    </row>
+    <row r="9" spans="1:20" ht="31.5" customHeight="1" outlineLevel="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="141" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="142"/>
-      <c r="D9" s="142"/>
-      <c r="E9" s="142"/>
-      <c r="F9" s="142"/>
-      <c r="G9" s="142"/>
-      <c r="H9" s="142"/>
-      <c r="I9" s="142"/>
-      <c r="J9" s="142"/>
-      <c r="K9" s="143"/>
-    </row>
-    <row r="10" spans="1:11" ht="19.8" customHeight="1" outlineLevel="1" thickBot="1">
-      <c r="B10" s="144" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="145"/>
-      <c r="D10" s="145"/>
-      <c r="E10" s="145"/>
-      <c r="F10" s="145"/>
-      <c r="G10" s="145"/>
-      <c r="H10" s="145"/>
-      <c r="I10" s="145"/>
-      <c r="J10" s="145"/>
-      <c r="K10" s="146"/>
-    </row>
-    <row r="11" spans="1:11" ht="15" outlineLevel="1" thickBot="1">
+      <c r="B9" s="192" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="193"/>
+      <c r="D9" s="193"/>
+      <c r="E9" s="193"/>
+      <c r="F9" s="193"/>
+      <c r="G9" s="193"/>
+      <c r="H9" s="193"/>
+      <c r="I9" s="193"/>
+      <c r="J9" s="193"/>
+      <c r="K9" s="194"/>
+    </row>
+    <row r="10" spans="1:20" ht="19.75" customHeight="1" outlineLevel="1" thickBot="1">
+      <c r="B10" s="195" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="196"/>
+      <c r="D10" s="196"/>
+      <c r="E10" s="196"/>
+      <c r="F10" s="196"/>
+      <c r="G10" s="196"/>
+      <c r="H10" s="196"/>
+      <c r="I10" s="196"/>
+      <c r="J10" s="196"/>
+      <c r="K10" s="197"/>
+    </row>
+    <row r="11" spans="1:20" ht="15" outlineLevel="1" thickBot="1">
       <c r="A11" s="2"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="38"/>
-    </row>
-    <row r="12" spans="1:11" ht="27" thickBot="1">
+      <c r="B11" s="54"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="59"/>
+      <c r="K11" s="60"/>
+    </row>
+    <row r="12" spans="1:20" ht="41.6" thickBot="1">
       <c r="A12" s="3"/>
-      <c r="B12" s="63" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="64" t="s">
+      <c r="B12" s="85" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="64" t="s">
+      <c r="D12" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="64" t="s">
+      <c r="E12" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="64" t="s">
+      <c r="F12" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="77" t="s">
+      <c r="G12" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="77" t="s">
+      <c r="H12" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="I12" s="77" t="s">
+      <c r="I12" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="J12" s="77" t="s">
+      <c r="J12" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="K12" s="77" t="s">
+      <c r="K12" s="99" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="10.050000000000001" customHeight="1" thickBot="1">
+      <c r="L12" s="29"/>
+      <c r="M12" s="152" t="s">
+        <v>52</v>
+      </c>
+      <c r="N12" s="152" t="s">
+        <v>53</v>
+      </c>
+      <c r="O12" s="152" t="s">
+        <v>54</v>
+      </c>
+      <c r="P12" s="152" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q12" s="153" t="s">
+        <v>38</v>
+      </c>
+      <c r="R12" s="152" t="s">
+        <v>81</v>
+      </c>
+      <c r="S12" s="153" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="10" customHeight="1" thickBot="1">
       <c r="A13" s="3"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="41"/>
-    </row>
-    <row r="14" spans="1:11" ht="20.25" customHeight="1" thickBot="1">
-      <c r="B14" s="85" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="86"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="133"/>
-      <c r="G14" s="86"/>
-      <c r="H14" s="86"/>
-      <c r="I14" s="86"/>
-      <c r="J14" s="86"/>
-      <c r="K14" s="87"/>
-    </row>
-    <row r="15" spans="1:11" ht="20.100000000000001" customHeight="1">
-      <c r="B15" s="42">
-        <v>1</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="15">
+      <c r="B13" s="61"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="35"/>
+      <c r="O13" s="35"/>
+      <c r="P13" s="35"/>
+      <c r="Q13" s="36"/>
+      <c r="R13" s="36"/>
+      <c r="S13" s="36"/>
+      <c r="T13" s="36"/>
+    </row>
+    <row r="14" spans="1:20" ht="20.25" customHeight="1" thickBot="1">
+      <c r="B14" s="107" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="108"/>
+      <c r="D14" s="108"/>
+      <c r="E14" s="108"/>
+      <c r="F14" s="166"/>
+      <c r="G14" s="108"/>
+      <c r="H14" s="108"/>
+      <c r="I14" s="108"/>
+      <c r="J14" s="108"/>
+      <c r="K14" s="109"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="37"/>
+      <c r="Q14" s="38"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="22"/>
+      <c r="T14" s="22"/>
+    </row>
+    <row r="15" spans="1:20" ht="20.149999999999999" customHeight="1">
+      <c r="B15" s="64">
+        <v>1</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="21">
         <v>1700</v>
       </c>
-      <c r="F15" s="9" t="e">
-        <f>#REF!*#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G15" s="9" t="e">
-        <f t="shared" ref="G15:G16" si="0">F15*E15</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H15" s="15">
+      <c r="F15" s="15">
+        <f t="shared" ref="F15:F24" si="0">N15*M15</f>
+        <v>1.1375</v>
+      </c>
+      <c r="G15" s="15">
+        <f t="shared" ref="G15:G16" si="1">F15*E15</f>
+        <v>1933.75</v>
+      </c>
+      <c r="H15" s="21">
         <f>E15</f>
         <v>1700</v>
       </c>
-      <c r="I15" s="9">
-        <v>1</v>
-      </c>
-      <c r="J15" s="9">
-        <f t="shared" ref="J15:J16" si="1">I15*H15</f>
+      <c r="I15" s="15">
+        <v>1</v>
+      </c>
+      <c r="J15" s="15">
+        <f t="shared" ref="J15:J16" si="2">I15*H15</f>
         <v>1700</v>
       </c>
-      <c r="K15" s="124" t="e">
+      <c r="K15" s="148">
         <f>G15+J15</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="20.100000000000001" customHeight="1">
-      <c r="B16" s="42">
-        <f t="shared" ref="B16:B17" si="2">B15+1</f>
+        <v>3633.75</v>
+      </c>
+      <c r="L15" s="157"/>
+      <c r="M15" s="23">
+        <v>1</v>
+      </c>
+      <c r="N15" s="198">
+        <v>1.1375</v>
+      </c>
+      <c r="O15" s="23">
+        <f>N15*E15</f>
+        <v>1933.75</v>
+      </c>
+      <c r="P15" s="23">
+        <f>G15-O15</f>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="147">
+        <f>P15/G15</f>
+        <v>0</v>
+      </c>
+      <c r="R15" t="b">
+        <f>AND(G15=E15*F15,F15=N15*M15,O15=E15*N15,P15=G15-O15,H15=E15,Q15=P15/G15,K15=J15+G15,J15=I15*H15)</f>
+        <v>1</v>
+      </c>
+      <c r="S15" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="T15" s="22"/>
+    </row>
+    <row r="16" spans="1:20" ht="20.149999999999999" customHeight="1">
+      <c r="B16" s="64">
+        <f t="shared" ref="B16:B17" si="3">B15+1</f>
         <v>2</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="13" t="s">
+      <c r="C16" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E16" s="15">
-        <v>1</v>
-      </c>
-      <c r="F16" s="9" t="e">
-        <f>#REF!*#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G16" s="9" t="e">
+      <c r="E16" s="21">
+        <v>1</v>
+      </c>
+      <c r="F16" s="15">
         <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="H16" s="15">
+        <v>196.875</v>
+      </c>
+      <c r="G16" s="15">
+        <f t="shared" si="1"/>
+        <v>196.875</v>
+      </c>
+      <c r="H16" s="21">
         <f>E16</f>
         <v>1</v>
       </c>
-      <c r="I16" s="9">
-        <v>1</v>
-      </c>
-      <c r="J16" s="9">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K16" s="124" t="e">
+      <c r="I16" s="15">
+        <v>1</v>
+      </c>
+      <c r="J16" s="15">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K16" s="148">
         <f>G16+J16</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:30" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B17" s="69">
-        <f t="shared" si="2"/>
+        <v>197.875</v>
+      </c>
+      <c r="L16" s="157"/>
+      <c r="M16" s="23">
+        <v>1</v>
+      </c>
+      <c r="N16" s="198">
+        <v>196.875</v>
+      </c>
+      <c r="O16" s="23">
+        <f>N16*E16</f>
+        <v>196.875</v>
+      </c>
+      <c r="P16" s="23">
+        <f>G16-O16</f>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="147">
+        <f>P16/G16</f>
+        <v>0</v>
+      </c>
+      <c r="R16" t="b">
+        <f t="shared" ref="R16:R17" si="4">AND(G16=E16*F16,F16=N16*M16,O16=E16*N16,P16=G16-O16,H16=E16,Q16=P16/G16,K16=J16+G16,J16=I16*H16)</f>
+        <v>1</v>
+      </c>
+      <c r="S16" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="T16" s="22"/>
+    </row>
+    <row r="17" spans="1:39" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="B17" s="91">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="C17" s="70" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="71" t="s">
+      <c r="C17" s="92" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="E17" s="72">
-        <v>1</v>
-      </c>
-      <c r="F17" s="73" t="e">
-        <f>#REF!*#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G17" s="73" t="e">
-        <f t="shared" ref="G17" si="3">F17*E17</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H17" s="72">
+      <c r="E17" s="94">
+        <v>1</v>
+      </c>
+      <c r="F17" s="95">
+        <f t="shared" si="0"/>
+        <v>1.2375</v>
+      </c>
+      <c r="G17" s="95">
+        <f t="shared" ref="G17" si="5">F17*E17</f>
+        <v>1.2375</v>
+      </c>
+      <c r="H17" s="94">
         <f>E17</f>
         <v>1</v>
       </c>
-      <c r="I17" s="73">
-        <v>1</v>
-      </c>
-      <c r="J17" s="73">
-        <f t="shared" ref="J17" si="4">I17*H17</f>
-        <v>1</v>
-      </c>
-      <c r="K17" s="125" t="e">
+      <c r="I17" s="95">
+        <v>1</v>
+      </c>
+      <c r="J17" s="95">
+        <f t="shared" ref="J17" si="6">I17*H17</f>
+        <v>1</v>
+      </c>
+      <c r="K17" s="149">
         <f>G17+J17</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:30" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B18" s="88" t="str">
+        <v>2.2374999999999998</v>
+      </c>
+      <c r="L17" s="157"/>
+      <c r="M17" s="23">
+        <v>1</v>
+      </c>
+      <c r="N17" s="198">
+        <v>1.2375</v>
+      </c>
+      <c r="O17" s="23">
+        <f>N17*E17</f>
+        <v>1.2375</v>
+      </c>
+      <c r="P17" s="23">
+        <f>G17-O17</f>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="147">
+        <f>P17/G17</f>
+        <v>0</v>
+      </c>
+      <c r="R17" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="S17" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="T17" s="22"/>
+    </row>
+    <row r="18" spans="1:39" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="B18" s="110" t="str">
         <f>B14 &amp; " SPOLU:"</f>
         <v>Optický kábel SPOLU:</v>
       </c>
-      <c r="C18" s="89"/>
-      <c r="D18" s="89"/>
-      <c r="E18" s="90"/>
-      <c r="F18" s="74" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" s="75" t="e">
+      <c r="C18" s="111"/>
+      <c r="D18" s="111"/>
+      <c r="E18" s="112"/>
+      <c r="F18" s="96" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="97">
         <f>SUM(G15:G17)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H18" s="83"/>
-      <c r="I18" s="74" t="s">
-        <v>37</v>
-      </c>
-      <c r="J18" s="75">
+        <v>2131.8625000000002</v>
+      </c>
+      <c r="H18" s="105"/>
+      <c r="I18" s="96" t="s">
+        <v>61</v>
+      </c>
+      <c r="J18" s="97">
         <f>SUM(J15:J17)</f>
         <v>1702</v>
       </c>
-      <c r="K18" s="82" t="e">
+      <c r="K18" s="104">
         <f>ROUNDUP(SUM(K15:K17),0)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:30" ht="10.050000000000001" customHeight="1" thickBot="1">
-      <c r="B19" s="43"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="46"/>
-      <c r="K19" s="47"/>
-    </row>
-    <row r="20" spans="1:30" ht="20.25" customHeight="1" thickBot="1">
-      <c r="B20" s="129" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="130"/>
-      <c r="D20" s="130"/>
-      <c r="E20" s="130"/>
-      <c r="F20" s="131"/>
-      <c r="G20" s="130"/>
-      <c r="H20" s="130"/>
-      <c r="I20" s="130"/>
-      <c r="J20" s="130"/>
-      <c r="K20" s="132"/>
-    </row>
-    <row r="21" spans="1:30" s="5" customFormat="1" ht="20.25" customHeight="1">
+        <v>3834</v>
+      </c>
+      <c r="L18" s="157"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="198"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="147"/>
+      <c r="R18" s="167"/>
+      <c r="S18" s="22"/>
+      <c r="T18" s="22"/>
+    </row>
+    <row r="19" spans="1:39" ht="10" customHeight="1" thickBot="1">
+      <c r="B19" s="65"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="68"/>
+      <c r="H19" s="66"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="68"/>
+      <c r="K19" s="69"/>
+      <c r="L19" s="157"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="198"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="147"/>
+      <c r="R19" s="167"/>
+      <c r="S19" s="22"/>
+      <c r="T19" s="22"/>
+    </row>
+    <row r="20" spans="1:39" ht="20.25" customHeight="1" thickBot="1">
+      <c r="B20" s="162" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="163"/>
+      <c r="D20" s="163"/>
+      <c r="E20" s="163"/>
+      <c r="F20" s="164"/>
+      <c r="G20" s="163"/>
+      <c r="H20" s="163"/>
+      <c r="I20" s="163"/>
+      <c r="J20" s="163"/>
+      <c r="K20" s="165"/>
+      <c r="L20" s="157"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="198"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="147"/>
+      <c r="R20" s="167"/>
+      <c r="S20" s="22"/>
+      <c r="T20" s="22"/>
+    </row>
+    <row r="21" spans="1:39" s="5" customFormat="1" ht="20.25" customHeight="1">
       <c r="A21" s="4"/>
-      <c r="B21" s="48">
+      <c r="B21" s="70">
         <f>B17+1</f>
         <v>4</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E21" s="11">
-        <v>1</v>
-      </c>
-      <c r="F21" s="12" t="e">
-        <f>#REF!*#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G21" s="12" t="e">
+      <c r="E21" s="17">
+        <v>1</v>
+      </c>
+      <c r="F21" s="18">
+        <f t="shared" si="0"/>
+        <v>687.625</v>
+      </c>
+      <c r="G21" s="18">
         <f>F21*E21</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H21" s="11">
+        <v>687.625</v>
+      </c>
+      <c r="H21" s="17">
         <f>E21</f>
         <v>1</v>
       </c>
-      <c r="I21" s="12">
-        <v>1</v>
-      </c>
-      <c r="J21" s="12">
-        <f t="shared" ref="J21:J23" si="5">I21*H21</f>
-        <v>1</v>
-      </c>
-      <c r="K21" s="124" t="e">
+      <c r="I21" s="18">
+        <v>1</v>
+      </c>
+      <c r="J21" s="18">
+        <f t="shared" ref="J21:J23" si="7">I21*H21</f>
+        <v>1</v>
+      </c>
+      <c r="K21" s="148">
         <f>G21+J21</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L21"/>
-      <c r="M21"/>
-      <c r="N21"/>
-      <c r="O21"/>
-      <c r="P21"/>
-    </row>
-    <row r="22" spans="1:30" s="5" customFormat="1" ht="20.25" customHeight="1">
+        <v>688.625</v>
+      </c>
+      <c r="L21" s="157"/>
+      <c r="M21" s="23">
+        <v>1</v>
+      </c>
+      <c r="N21" s="198">
+        <v>687.625</v>
+      </c>
+      <c r="O21" s="23">
+        <f>E21*N21</f>
+        <v>687.625</v>
+      </c>
+      <c r="P21" s="23">
+        <f>G21-O21</f>
+        <v>0</v>
+      </c>
+      <c r="Q21" s="147">
+        <f>P21/G21</f>
+        <v>0</v>
+      </c>
+      <c r="R21" t="b">
+        <f t="shared" ref="R21:R24" si="8">AND(G21=E21*F21,F21=N21*M21,O21=E21*N21,P21=G21-O21,H21=E21,Q21=P21/G21,K21=J21+G21,J21=I21*H21)</f>
+        <v>1</v>
+      </c>
+      <c r="S21" s="24"/>
+      <c r="T21" s="4"/>
+      <c r="U21"/>
+      <c r="V21"/>
+      <c r="W21"/>
+      <c r="X21"/>
+      <c r="Y21"/>
+    </row>
+    <row r="22" spans="1:39" s="5" customFormat="1" ht="20.25" customHeight="1">
       <c r="A22" s="4"/>
-      <c r="B22" s="42">
-        <f t="shared" ref="B22:B24" si="6">B21+1</f>
+      <c r="B22" s="64">
+        <f t="shared" ref="B22:B24" si="9">B21+1</f>
         <v>5</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E22" s="15">
-        <v>1</v>
-      </c>
-      <c r="F22" s="9" t="e">
-        <f>#REF!*#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G22" s="9" t="e">
-        <f t="shared" ref="G22:G23" si="7">F22*E22</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H22" s="15">
+      <c r="E22" s="21">
+        <v>1</v>
+      </c>
+      <c r="F22" s="15">
+        <f t="shared" si="0"/>
+        <v>158.66250000000002</v>
+      </c>
+      <c r="G22" s="15">
+        <f t="shared" ref="G22:G23" si="10">F22*E22</f>
+        <v>158.66250000000002</v>
+      </c>
+      <c r="H22" s="21">
         <f>E22</f>
         <v>1</v>
       </c>
-      <c r="I22" s="9">
-        <v>1</v>
-      </c>
-      <c r="J22" s="9">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="K22" s="124" t="e">
+      <c r="I22" s="15">
+        <v>1</v>
+      </c>
+      <c r="J22" s="15">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="K22" s="148">
         <f>G22+J22</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M22" s="8"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-    </row>
-    <row r="23" spans="1:30" s="5" customFormat="1" ht="20.25" customHeight="1">
+        <v>159.66250000000002</v>
+      </c>
+      <c r="L22" s="157"/>
+      <c r="M22" s="23">
+        <v>1</v>
+      </c>
+      <c r="N22" s="198">
+        <v>158.66250000000002</v>
+      </c>
+      <c r="O22" s="23">
+        <f>E22*N22</f>
+        <v>158.66250000000002</v>
+      </c>
+      <c r="P22" s="23">
+        <f>G22-O22</f>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="147">
+        <f>P22/G22</f>
+        <v>0</v>
+      </c>
+      <c r="R22" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="S22" s="25"/>
+      <c r="T22" s="4"/>
+      <c r="V22" s="8"/>
+      <c r="X22" s="4"/>
+      <c r="Y22" s="4"/>
+    </row>
+    <row r="23" spans="1:39" s="5" customFormat="1" ht="20.25" customHeight="1">
       <c r="A23" s="4"/>
-      <c r="B23" s="42">
-        <f t="shared" si="6"/>
+      <c r="B23" s="64">
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E23" s="15">
-        <v>1</v>
-      </c>
-      <c r="F23" s="9" t="e">
-        <f>#REF!*#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G23" s="9" t="e">
+      <c r="E23" s="21">
+        <v>1</v>
+      </c>
+      <c r="F23" s="15">
+        <f t="shared" si="0"/>
+        <v>126.0625</v>
+      </c>
+      <c r="G23" s="15">
+        <f t="shared" si="10"/>
+        <v>126.0625</v>
+      </c>
+      <c r="H23" s="21">
+        <f>E23</f>
+        <v>1</v>
+      </c>
+      <c r="I23" s="15">
+        <v>1</v>
+      </c>
+      <c r="J23" s="15">
         <f t="shared" si="7"/>
-        <v>#REF!</v>
-      </c>
-      <c r="H23" s="15">
-        <f>E23</f>
-        <v>1</v>
-      </c>
-      <c r="I23" s="9">
-        <v>1</v>
-      </c>
-      <c r="J23" s="9">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="K23" s="125" t="e">
+        <v>1</v>
+      </c>
+      <c r="K23" s="149">
         <f>G23+J23</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
-      <c r="R23" s="4"/>
-      <c r="S23" s="4"/>
+        <v>127.0625</v>
+      </c>
+      <c r="L23" s="157"/>
+      <c r="M23" s="23">
+        <v>1</v>
+      </c>
+      <c r="N23" s="198">
+        <v>126.0625</v>
+      </c>
+      <c r="O23" s="23">
+        <f>E23*N23</f>
+        <v>126.0625</v>
+      </c>
+      <c r="P23" s="23">
+        <f>G23-O23</f>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="147">
+        <f>P23/G23</f>
+        <v>0</v>
+      </c>
+      <c r="R23" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="S23" s="24"/>
       <c r="T23" s="4"/>
-      <c r="U23" s="4"/>
-      <c r="V23" s="4"/>
-      <c r="W23" s="7"/>
-      <c r="X23" s="6"/>
+      <c r="X23" s="4"/>
       <c r="Y23" s="4"/>
-      <c r="Z23" s="4"/>
       <c r="AA23" s="4"/>
       <c r="AB23" s="4"/>
       <c r="AC23" s="4"/>
       <c r="AD23" s="4"/>
-    </row>
-    <row r="24" spans="1:30" ht="20.25" customHeight="1" thickBot="1">
-      <c r="B24" s="69">
-        <f t="shared" si="6"/>
+      <c r="AE23" s="4"/>
+      <c r="AF23" s="7"/>
+      <c r="AG23" s="6"/>
+      <c r="AH23" s="4"/>
+      <c r="AI23" s="4"/>
+      <c r="AJ23" s="4"/>
+      <c r="AK23" s="4"/>
+      <c r="AL23" s="4"/>
+      <c r="AM23" s="4"/>
+    </row>
+    <row r="24" spans="1:39" ht="20.25" customHeight="1" thickBot="1">
+      <c r="B24" s="91">
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
-      <c r="C24" s="70" t="s">
+      <c r="C24" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="71" t="s">
+      <c r="D24" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="72">
+      <c r="E24" s="94">
         <v>100</v>
       </c>
-      <c r="F24" s="73" t="e">
-        <f>#REF!*#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G24" s="73" t="e">
-        <f t="shared" ref="G24" si="8">F24*E24</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H24" s="72">
+      <c r="F24" s="95">
+        <f t="shared" si="0"/>
+        <v>124.3</v>
+      </c>
+      <c r="G24" s="95">
+        <f t="shared" ref="G24" si="11">F24*E24</f>
+        <v>12430</v>
+      </c>
+      <c r="H24" s="94">
         <f>E24</f>
         <v>100</v>
       </c>
-      <c r="I24" s="73">
-        <v>1</v>
-      </c>
-      <c r="J24" s="73">
-        <f t="shared" ref="J24" si="9">I24*H24</f>
+      <c r="I24" s="95">
+        <v>1</v>
+      </c>
+      <c r="J24" s="95">
+        <f t="shared" ref="J24" si="12">I24*H24</f>
         <v>100</v>
       </c>
-      <c r="K24" s="124" t="e">
+      <c r="K24" s="148">
         <f>G24+J24</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="25" spans="1:30" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B25" s="88" t="str">
+        <v>12530</v>
+      </c>
+      <c r="L24" s="157"/>
+      <c r="M24" s="23">
+        <v>1</v>
+      </c>
+      <c r="N24" s="198">
+        <v>124.3</v>
+      </c>
+      <c r="O24" s="23">
+        <f>E24*N24</f>
+        <v>12430</v>
+      </c>
+      <c r="P24" s="23">
+        <f>G24-O24</f>
+        <v>0</v>
+      </c>
+      <c r="Q24" s="147">
+        <f>P24/G24</f>
+        <v>0</v>
+      </c>
+      <c r="R24" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="S24" s="22"/>
+      <c r="T24" s="22"/>
+    </row>
+    <row r="25" spans="1:39" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="B25" s="110" t="str">
         <f>B20 &amp; " SPOLU:"</f>
         <v>Prístupový a zabezpečovací systém (ACS/EZS) SPOLU:</v>
       </c>
-      <c r="C25" s="89"/>
-      <c r="D25" s="89"/>
-      <c r="E25" s="90"/>
-      <c r="F25" s="74" t="s">
-        <v>38</v>
-      </c>
-      <c r="G25" s="75" t="e">
+      <c r="C25" s="111"/>
+      <c r="D25" s="111"/>
+      <c r="E25" s="112"/>
+      <c r="F25" s="96" t="s">
+        <v>62</v>
+      </c>
+      <c r="G25" s="97">
         <f>SUM(G21:G24)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H25" s="83"/>
-      <c r="I25" s="74" t="s">
-        <v>37</v>
-      </c>
-      <c r="J25" s="75">
+        <v>13402.35</v>
+      </c>
+      <c r="H25" s="105"/>
+      <c r="I25" s="96" t="s">
+        <v>61</v>
+      </c>
+      <c r="J25" s="97">
         <f>SUM(J21:J24)</f>
         <v>103</v>
       </c>
-      <c r="K25" s="82" t="e">
+      <c r="K25" s="104">
         <f>ROUNDUP(SUM(K21:K24),0)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="26" spans="1:30" ht="10.050000000000001" customHeight="1" thickBot="1">
-      <c r="B26" s="49"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="80"/>
-      <c r="G26" s="81"/>
-      <c r="H26" s="50"/>
-      <c r="I26" s="51"/>
-      <c r="J26" s="52"/>
-      <c r="K26" s="53"/>
-    </row>
-    <row r="27" spans="1:30" ht="20.25" customHeight="1" thickBot="1">
-      <c r="B27" s="85" t="s">
+        <v>13506</v>
+      </c>
+      <c r="L25" s="29"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="22"/>
+      <c r="O25" s="22"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="22"/>
+    </row>
+    <row r="26" spans="1:39" ht="10" customHeight="1" thickBot="1">
+      <c r="B26" s="71"/>
+      <c r="C26" s="72"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="72"/>
+      <c r="F26" s="102"/>
+      <c r="G26" s="103"/>
+      <c r="H26" s="72"/>
+      <c r="I26" s="73"/>
+      <c r="J26" s="74"/>
+      <c r="K26" s="75"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="22"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="22"/>
+    </row>
+    <row r="27" spans="1:39" ht="20.25" customHeight="1" thickBot="1">
+      <c r="B27" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="86"/>
-      <c r="D27" s="86"/>
-      <c r="E27" s="84"/>
-      <c r="F27" s="86"/>
-      <c r="G27" s="86"/>
-      <c r="H27" s="86"/>
-      <c r="I27" s="86"/>
-      <c r="J27" s="86"/>
-      <c r="K27" s="87"/>
-    </row>
-    <row r="28" spans="1:30" ht="20.100000000000001" customHeight="1">
-      <c r="B28" s="48">
+      <c r="C27" s="108"/>
+      <c r="D27" s="108"/>
+      <c r="E27" s="106"/>
+      <c r="F27" s="108"/>
+      <c r="G27" s="108"/>
+      <c r="H27" s="108"/>
+      <c r="I27" s="108"/>
+      <c r="J27" s="108"/>
+      <c r="K27" s="109"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="22"/>
+      <c r="T27" s="22"/>
+    </row>
+    <row r="28" spans="1:39" ht="20.149999999999999" customHeight="1">
+      <c r="B28" s="70">
         <f>B24+1</f>
         <v>8</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="E28" s="11"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="11">
+      <c r="D28" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" s="17"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="17">
         <v>12</v>
       </c>
-      <c r="I28" s="12">
-        <v>1</v>
-      </c>
-      <c r="J28" s="12">
-        <f t="shared" ref="J28" si="10">I28*H28</f>
+      <c r="I28" s="18">
+        <v>1</v>
+      </c>
+      <c r="J28" s="18">
+        <f t="shared" ref="J28" si="13">I28*H28</f>
         <v>12</v>
       </c>
-      <c r="K28" s="124">
-        <f t="shared" ref="K28:K34" si="11">G28+J28</f>
+      <c r="K28" s="148">
+        <f t="shared" ref="K28:K34" si="14">G28+J28</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="1:30" ht="20.100000000000001" customHeight="1">
-      <c r="B29" s="42">
-        <f t="shared" ref="B29:B30" si="12">B28+1</f>
+      <c r="L28" s="29"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="22"/>
+      <c r="O28" s="22"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="22"/>
+    </row>
+    <row r="29" spans="1:39" ht="20.149999999999999" customHeight="1">
+      <c r="B29" s="64">
+        <f t="shared" ref="B29:B30" si="15">B28+1</f>
         <v>9</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="E29" s="15"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="15">
+      <c r="D29" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29" s="21"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="21">
         <v>12</v>
       </c>
-      <c r="I29" s="9">
-        <v>1</v>
-      </c>
-      <c r="J29" s="9">
-        <f t="shared" ref="J29:J30" si="13">I29*H29</f>
+      <c r="I29" s="15">
+        <v>1</v>
+      </c>
+      <c r="J29" s="15">
+        <f t="shared" ref="J29:J30" si="16">I29*H29</f>
         <v>12</v>
       </c>
-      <c r="K29" s="124">
-        <f t="shared" si="11"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:30" ht="20.100000000000001" customHeight="1">
-      <c r="B30" s="42">
-        <f t="shared" si="12"/>
-        <v>10</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E30" s="15"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="15">
-        <v>1</v>
-      </c>
-      <c r="I30" s="9">
-        <v>1</v>
-      </c>
-      <c r="J30" s="9">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="K30" s="125">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:30" ht="20.100000000000001" customHeight="1">
-      <c r="B31" s="42">
-        <f t="shared" ref="B31:B34" si="14">B30+1</f>
-        <v>11</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E31" s="15"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="15">
-        <v>5</v>
-      </c>
-      <c r="I31" s="9" t="e">
-        <f>K18+K25</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J31" s="9" t="e">
-        <f>I31*H31%</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K31" s="124" t="e">
-        <f t="shared" si="11"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="32" spans="1:30" ht="20.100000000000001" customHeight="1">
-      <c r="B32" s="42">
+      <c r="K29" s="148">
         <f t="shared" si="14"/>
         <v>12</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="L29" s="29"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="22"/>
+      <c r="O29" s="22"/>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="22"/>
+      <c r="R29" s="22"/>
+      <c r="S29" s="22"/>
+      <c r="T29" s="22"/>
+    </row>
+    <row r="30" spans="1:39" ht="20.149999999999999" customHeight="1">
+      <c r="B30" s="64">
+        <f t="shared" si="15"/>
+        <v>10</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" s="21"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="21">
+        <v>1</v>
+      </c>
+      <c r="I30" s="15">
+        <v>1</v>
+      </c>
+      <c r="J30" s="15">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="K30" s="149">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="L30" s="29"/>
+      <c r="M30" s="22"/>
+      <c r="N30" s="22"/>
+      <c r="O30" s="22"/>
+      <c r="P30" s="33"/>
+      <c r="Q30" s="22"/>
+      <c r="R30" s="22"/>
+      <c r="S30" s="22"/>
+      <c r="T30" s="22"/>
+    </row>
+    <row r="31" spans="1:39" ht="20.149999999999999" customHeight="1">
+      <c r="B31" s="64">
+        <f t="shared" ref="B31:B34" si="17">B30+1</f>
+        <v>11</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" s="21"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="21">
+        <v>5</v>
+      </c>
+      <c r="I31" s="15">
+        <f>K18+K25</f>
+        <v>17340</v>
+      </c>
+      <c r="J31" s="15">
+        <f>I31*H31%</f>
+        <v>867</v>
+      </c>
+      <c r="K31" s="148">
+        <f t="shared" si="14"/>
+        <v>867</v>
+      </c>
+      <c r="L31" s="40"/>
+      <c r="M31" s="22"/>
+      <c r="N31" s="22"/>
+      <c r="O31" s="22"/>
+      <c r="P31" s="22"/>
+      <c r="Q31" s="22"/>
+      <c r="R31" s="22"/>
+      <c r="S31" s="22"/>
+      <c r="T31" s="22"/>
+    </row>
+    <row r="32" spans="1:39" ht="20.149999999999999" customHeight="1">
+      <c r="B32" s="64">
+        <f t="shared" si="17"/>
+        <v>12</v>
+      </c>
+      <c r="C32" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D32" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E32" s="15"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="15">
+      <c r="D32" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32" s="21"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="21">
         <v>3</v>
       </c>
-      <c r="I32" s="9">
+      <c r="I32" s="15">
         <f>J18+J25</f>
         <v>1805</v>
       </c>
-      <c r="J32" s="9">
+      <c r="J32" s="15">
         <f>I32*H32%</f>
         <v>54.15</v>
       </c>
-      <c r="K32" s="124">
-        <f t="shared" si="11"/>
+      <c r="K32" s="148">
+        <f t="shared" si="14"/>
         <v>54.15</v>
       </c>
-    </row>
-    <row r="33" spans="2:11">
-      <c r="B33" s="42">
+      <c r="L32" s="40"/>
+      <c r="M32" s="22"/>
+      <c r="N32" s="22"/>
+      <c r="O32" s="22"/>
+      <c r="P32" s="22"/>
+      <c r="Q32" s="22"/>
+      <c r="R32" s="22"/>
+      <c r="S32" s="22"/>
+      <c r="T32" s="22"/>
+    </row>
+    <row r="33" spans="2:20" ht="28.3">
+      <c r="B33" s="64">
+        <f t="shared" si="17"/>
+        <v>13</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="E33" s="21"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="21">
+        <v>1</v>
+      </c>
+      <c r="I33" s="15">
+        <v>1</v>
+      </c>
+      <c r="J33" s="15">
+        <f t="shared" ref="J33:J34" si="18">I33*H33</f>
+        <v>1</v>
+      </c>
+      <c r="K33" s="148">
         <f t="shared" si="14"/>
-        <v>13</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E33" s="15"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="15">
-        <v>1</v>
-      </c>
-      <c r="I33" s="9">
-        <v>1</v>
-      </c>
-      <c r="J33" s="9">
-        <f t="shared" ref="J33:J34" si="15">I33*H33</f>
-        <v>1</v>
-      </c>
-      <c r="K33" s="124">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B34" s="69">
+        <v>1</v>
+      </c>
+      <c r="L33" s="29"/>
+      <c r="M33" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="N33" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="O33" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="P33" s="22"/>
+      <c r="Q33" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="R33" s="28"/>
+      <c r="S33" s="22"/>
+      <c r="T33" s="22"/>
+    </row>
+    <row r="34" spans="2:20" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="B34" s="91">
+        <f t="shared" si="17"/>
+        <v>14</v>
+      </c>
+      <c r="C34" s="92" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="93" t="s">
+        <v>83</v>
+      </c>
+      <c r="E34" s="94"/>
+      <c r="F34" s="95"/>
+      <c r="G34" s="95"/>
+      <c r="H34" s="94">
+        <v>1</v>
+      </c>
+      <c r="I34" s="95">
+        <v>1</v>
+      </c>
+      <c r="J34" s="95">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="K34" s="149">
         <f t="shared" si="14"/>
-        <v>14</v>
-      </c>
-      <c r="C34" s="70" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="71" t="s">
-        <v>53</v>
-      </c>
-      <c r="E34" s="72"/>
-      <c r="F34" s="73"/>
-      <c r="G34" s="73"/>
-      <c r="H34" s="72">
-        <v>1</v>
-      </c>
-      <c r="I34" s="73">
-        <v>1</v>
-      </c>
-      <c r="J34" s="73">
-        <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="K34" s="125">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="2:11" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B35" s="88" t="str">
+        <v>1</v>
+      </c>
+      <c r="L34" s="29"/>
+      <c r="M34" s="27">
+        <v>10</v>
+      </c>
+      <c r="N34" s="27">
+        <v>1</v>
+      </c>
+      <c r="O34" s="27">
+        <f>M34*N34</f>
+        <v>10</v>
+      </c>
+      <c r="P34" s="22"/>
+      <c r="Q34" s="29">
+        <v>0.1</v>
+      </c>
+      <c r="R34" s="29"/>
+      <c r="S34" s="22"/>
+      <c r="T34" s="22"/>
+    </row>
+    <row r="35" spans="2:20" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="B35" s="110" t="str">
         <f>B27 &amp; " SPOLU:"</f>
         <v>Dokumentácia, projektový manažment, ostatné SPOLU:</v>
       </c>
-      <c r="C35" s="89"/>
-      <c r="D35" s="89"/>
-      <c r="E35" s="89"/>
-      <c r="F35" s="65" t="s">
-        <v>38</v>
-      </c>
-      <c r="G35" s="75">
+      <c r="C35" s="111"/>
+      <c r="D35" s="111"/>
+      <c r="E35" s="111"/>
+      <c r="F35" s="87" t="s">
+        <v>62</v>
+      </c>
+      <c r="G35" s="97">
         <f>SUM(G28:G34)</f>
         <v>0</v>
       </c>
-      <c r="H35" s="89"/>
-      <c r="I35" s="65" t="s">
-        <v>37</v>
-      </c>
-      <c r="J35" s="75" t="e">
+      <c r="H35" s="111"/>
+      <c r="I35" s="87" t="s">
+        <v>61</v>
+      </c>
+      <c r="J35" s="97">
         <f>SUM(J28:J34)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K35" s="82" t="e">
+        <v>948.15</v>
+      </c>
+      <c r="K35" s="104">
         <f>ROUNDUP(SUM(K28:K34),0)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11" ht="16.2" thickBot="1">
-      <c r="B36" s="54"/>
-      <c r="C36" s="55"/>
-      <c r="D36" s="55"/>
-      <c r="E36" s="55"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="16"/>
-      <c r="J36" s="16"/>
-      <c r="K36" s="56"/>
-    </row>
-    <row r="37" spans="2:11" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B37" s="68"/>
-      <c r="C37" s="76"/>
-      <c r="D37" s="91"/>
-      <c r="E37" s="92"/>
-      <c r="F37" s="65" t="s">
+        <v>949</v>
+      </c>
+      <c r="L35" s="22"/>
+      <c r="M35" s="22"/>
+      <c r="N35" s="22"/>
+      <c r="O35" s="22"/>
+      <c r="P35" s="22"/>
+      <c r="Q35" s="22"/>
+      <c r="R35" s="22"/>
+      <c r="S35" s="22"/>
+      <c r="T35" s="22"/>
+    </row>
+    <row r="36" spans="2:20" ht="15.9" thickBot="1">
+      <c r="B36" s="76"/>
+      <c r="C36" s="77"/>
+      <c r="D36" s="77"/>
+      <c r="E36" s="77"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="78"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="30"/>
+      <c r="N36" s="181" t="s">
+        <v>26</v>
+      </c>
+      <c r="O36" s="182"/>
+      <c r="P36" s="182"/>
+      <c r="Q36" s="182"/>
+      <c r="R36" s="30"/>
+      <c r="T36" s="22"/>
+    </row>
+    <row r="37" spans="2:20" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="B37" s="90"/>
+      <c r="C37" s="98"/>
+      <c r="D37" s="113"/>
+      <c r="E37" s="114"/>
+      <c r="F37" s="87" t="s">
+        <v>66</v>
+      </c>
+      <c r="G37" s="88">
+        <f>G18+G25+G35</f>
+        <v>15534.212500000001</v>
+      </c>
+      <c r="H37" s="124"/>
+      <c r="I37" s="87" t="s">
+        <v>67</v>
+      </c>
+      <c r="J37" s="88">
+        <f>J18+J25+J35</f>
+        <v>2753.15</v>
+      </c>
+      <c r="K37" s="89">
+        <f>K18+K25+K35</f>
+        <v>18289</v>
+      </c>
+      <c r="L37" s="22"/>
+      <c r="M37" s="30"/>
+      <c r="N37" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O37" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="P37" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q37" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="R37" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="T37" s="22"/>
+    </row>
+    <row r="38" spans="2:20" ht="15.9" thickBot="1">
+      <c r="B38" s="76"/>
+      <c r="C38" s="77"/>
+      <c r="D38" s="77"/>
+      <c r="E38" s="77"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="22"/>
+      <c r="K38" s="78"/>
+      <c r="L38" s="22"/>
+      <c r="M38" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="N38" s="154">
+        <v>1</v>
+      </c>
+      <c r="O38" s="155">
+        <v>8</v>
+      </c>
+      <c r="P38" s="156">
+        <v>5</v>
+      </c>
+      <c r="Q38" s="156">
+        <f>N38*(O38*P38)</f>
         <v>40</v>
       </c>
-      <c r="G37" s="66" t="e">
-        <f>G18+G25+G35</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H37" s="101"/>
-      <c r="I37" s="65" t="s">
-        <v>41</v>
-      </c>
-      <c r="J37" s="66" t="e">
-        <f>J18+J25+J35</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K37" s="67" t="e">
-        <f>K18+K25+K35</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11" ht="16.2" thickBot="1">
-      <c r="B38" s="54"/>
-      <c r="C38" s="55"/>
-      <c r="D38" s="55"/>
-      <c r="E38" s="55"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
-      <c r="I38" s="16"/>
-      <c r="J38" s="16"/>
-      <c r="K38" s="56"/>
-    </row>
-    <row r="39" spans="2:11" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B39" s="119" t="s">
+      <c r="R38" s="14">
+        <f>Q38*1.1</f>
+        <v>44</v>
+      </c>
+      <c r="T38" s="22"/>
+    </row>
+    <row r="39" spans="2:20" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="B39" s="142" t="s">
         <v>22</v>
       </c>
-      <c r="C39" s="120"/>
-      <c r="D39" s="121"/>
-      <c r="E39" s="121"/>
-      <c r="F39" s="121"/>
-      <c r="G39" s="121"/>
-      <c r="H39" s="121"/>
-      <c r="I39" s="121"/>
-      <c r="J39" s="122"/>
-      <c r="K39" s="102" t="s">
+      <c r="C39" s="143"/>
+      <c r="D39" s="144"/>
+      <c r="E39" s="144"/>
+      <c r="F39" s="144"/>
+      <c r="G39" s="144"/>
+      <c r="H39" s="144"/>
+      <c r="I39" s="144"/>
+      <c r="J39" s="145"/>
+      <c r="K39" s="125" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="40" spans="2:11" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B40" s="115" t="str">
+      <c r="L39" s="22"/>
+      <c r="M39" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="N39" s="154">
+        <v>2</v>
+      </c>
+      <c r="O39" s="155">
+        <v>16</v>
+      </c>
+      <c r="P39" s="156">
+        <v>10</v>
+      </c>
+      <c r="Q39" s="156">
+        <f>N39*(O39*P39)</f>
+        <v>320</v>
+      </c>
+      <c r="R39" s="14">
+        <f t="shared" ref="R39:R41" si="19">Q39*1.1</f>
+        <v>352</v>
+      </c>
+      <c r="T39" s="22"/>
+    </row>
+    <row r="40" spans="2:20" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="B40" s="138" t="str">
         <f>B18</f>
         <v>Optický kábel SPOLU:</v>
       </c>
-      <c r="C40" s="116"/>
-      <c r="D40" s="117"/>
-      <c r="E40" s="117"/>
-      <c r="F40" s="117"/>
-      <c r="G40" s="117"/>
-      <c r="H40" s="117"/>
-      <c r="I40" s="117"/>
-      <c r="J40" s="118"/>
-      <c r="K40" s="103" t="e">
+      <c r="C40" s="139"/>
+      <c r="D40" s="140"/>
+      <c r="E40" s="140"/>
+      <c r="F40" s="140"/>
+      <c r="G40" s="140"/>
+      <c r="H40" s="140"/>
+      <c r="I40" s="140"/>
+      <c r="J40" s="141"/>
+      <c r="K40" s="126">
         <f>K18</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="41" spans="2:11" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B41" s="115" t="str">
+        <v>3834</v>
+      </c>
+      <c r="L40" s="22"/>
+      <c r="M40" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="N40" s="154">
+        <v>1</v>
+      </c>
+      <c r="O40" s="155">
+        <v>8</v>
+      </c>
+      <c r="P40" s="156">
+        <v>15</v>
+      </c>
+      <c r="Q40" s="156">
+        <f>N40*(O40*P40)</f>
+        <v>120</v>
+      </c>
+      <c r="R40" s="14">
+        <f t="shared" si="19"/>
+        <v>132</v>
+      </c>
+      <c r="T40" s="22"/>
+    </row>
+    <row r="41" spans="2:20" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="B41" s="138" t="str">
         <f>B25</f>
         <v>Prístupový a zabezpečovací systém (ACS/EZS) SPOLU:</v>
       </c>
-      <c r="C41" s="116"/>
-      <c r="D41" s="117"/>
-      <c r="E41" s="117"/>
-      <c r="F41" s="117"/>
-      <c r="G41" s="117"/>
-      <c r="H41" s="117"/>
-      <c r="I41" s="117"/>
-      <c r="J41" s="118"/>
-      <c r="K41" s="103" t="e">
+      <c r="C41" s="139"/>
+      <c r="D41" s="140"/>
+      <c r="E41" s="140"/>
+      <c r="F41" s="140"/>
+      <c r="G41" s="140"/>
+      <c r="H41" s="140"/>
+      <c r="I41" s="140"/>
+      <c r="J41" s="141"/>
+      <c r="K41" s="126">
         <f>K25</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="42" spans="2:11" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B42" s="115" t="str">
+        <v>13506</v>
+      </c>
+      <c r="L41" s="22"/>
+      <c r="M41" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N41" s="154">
+        <v>1</v>
+      </c>
+      <c r="O41" s="155">
+        <v>8</v>
+      </c>
+      <c r="P41" s="156">
+        <v>20</v>
+      </c>
+      <c r="Q41" s="156">
+        <f>N41*(O41*P41)</f>
+        <v>160</v>
+      </c>
+      <c r="R41" s="14">
+        <f t="shared" si="19"/>
+        <v>176</v>
+      </c>
+      <c r="T41" s="22"/>
+    </row>
+    <row r="42" spans="2:20" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="B42" s="138" t="str">
         <f>B35</f>
         <v>Dokumentácia, projektový manažment, ostatné SPOLU:</v>
       </c>
-      <c r="C42" s="116"/>
-      <c r="D42" s="117"/>
-      <c r="E42" s="117"/>
-      <c r="F42" s="117"/>
-      <c r="G42" s="117"/>
-      <c r="H42" s="117"/>
-      <c r="I42" s="117"/>
-      <c r="J42" s="118"/>
-      <c r="K42" s="103" t="e">
+      <c r="C42" s="139"/>
+      <c r="D42" s="140"/>
+      <c r="E42" s="140"/>
+      <c r="F42" s="140"/>
+      <c r="G42" s="140"/>
+      <c r="H42" s="140"/>
+      <c r="I42" s="140"/>
+      <c r="J42" s="141"/>
+      <c r="K42" s="126">
         <f>K35</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="43" spans="2:11" ht="18" thickBot="1">
-      <c r="B43" s="68"/>
-      <c r="C43" s="91"/>
-      <c r="D43" s="91"/>
-      <c r="E43" s="91"/>
-      <c r="F43" s="91"/>
-      <c r="G43" s="91"/>
-      <c r="H43" s="91"/>
-      <c r="I43" s="87"/>
-      <c r="J43" s="123" t="s">
-        <v>49</v>
-      </c>
-      <c r="K43" s="93" t="e">
+        <v>949</v>
+      </c>
+      <c r="L42" s="22"/>
+      <c r="M42" s="190" t="s">
+        <v>34</v>
+      </c>
+      <c r="N42" s="179" t="s">
+        <v>65</v>
+      </c>
+      <c r="O42" s="175" t="s">
+        <v>59</v>
+      </c>
+      <c r="P42" s="173" t="s">
+        <v>35</v>
+      </c>
+      <c r="T42" s="22"/>
+    </row>
+    <row r="43" spans="2:20" ht="18" thickBot="1">
+      <c r="B43" s="90"/>
+      <c r="C43" s="113"/>
+      <c r="D43" s="113"/>
+      <c r="E43" s="113"/>
+      <c r="F43" s="113"/>
+      <c r="G43" s="113"/>
+      <c r="H43" s="113"/>
+      <c r="I43" s="109"/>
+      <c r="J43" s="146" t="s">
+        <v>78</v>
+      </c>
+      <c r="K43" s="115">
         <f>SUM(K40:K42)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="44" spans="2:11" ht="18" thickBot="1">
-      <c r="B44" s="78"/>
-      <c r="C44" s="94"/>
-      <c r="D44" s="94"/>
-      <c r="E44" s="94"/>
-      <c r="F44" s="94"/>
-      <c r="G44" s="94"/>
-      <c r="H44" s="94"/>
-      <c r="I44" s="95"/>
-      <c r="J44" s="95"/>
-      <c r="K44" s="96"/>
-    </row>
-    <row r="45" spans="2:11" ht="20.100000000000001" customHeight="1">
-      <c r="B45" s="104" t="s">
+        <v>18289</v>
+      </c>
+      <c r="L43" s="22"/>
+      <c r="M43" s="191"/>
+      <c r="N43" s="180"/>
+      <c r="O43" s="176"/>
+      <c r="P43" s="174"/>
+      <c r="T43" s="22"/>
+    </row>
+    <row r="44" spans="2:20" ht="18" thickBot="1">
+      <c r="B44" s="100"/>
+      <c r="C44" s="116"/>
+      <c r="D44" s="116"/>
+      <c r="E44" s="116"/>
+      <c r="F44" s="116"/>
+      <c r="G44" s="116"/>
+      <c r="H44" s="116"/>
+      <c r="I44" s="117"/>
+      <c r="J44" s="117"/>
+      <c r="K44" s="118"/>
+      <c r="L44" s="22"/>
+      <c r="M44" s="158">
+        <f>SUM(O15:O24)</f>
+        <v>15534.2125</v>
+      </c>
+      <c r="N44" s="158">
+        <f>G37</f>
+        <v>15534.212500000001</v>
+      </c>
+      <c r="O44" s="31">
+        <f>N44-M44</f>
+        <v>0</v>
+      </c>
+      <c r="P44" s="32">
+        <f>O44/N44</f>
+        <v>0</v>
+      </c>
+      <c r="T44" s="22"/>
+    </row>
+    <row r="45" spans="2:20" ht="20.149999999999999" customHeight="1">
+      <c r="B45" s="127" t="s">
         <v>8</v>
       </c>
-      <c r="C45" s="105"/>
-      <c r="D45" s="105"/>
-      <c r="E45" s="105"/>
-      <c r="F45" s="105"/>
-      <c r="G45" s="105"/>
-      <c r="H45" s="105"/>
-      <c r="I45" s="105"/>
-      <c r="J45" s="105"/>
-      <c r="K45" s="106"/>
-    </row>
-    <row r="46" spans="2:11" ht="15" customHeight="1">
-      <c r="B46" s="79">
-        <v>1</v>
-      </c>
-      <c r="C46" s="97" t="s">
-        <v>27</v>
-      </c>
-      <c r="D46" s="98"/>
-      <c r="E46" s="98"/>
-      <c r="F46" s="98"/>
-      <c r="G46" s="98"/>
-      <c r="H46" s="98"/>
-      <c r="I46" s="98"/>
-      <c r="J46" s="98"/>
-      <c r="K46" s="99"/>
-    </row>
-    <row r="47" spans="2:11" ht="15" customHeight="1">
-      <c r="B47" s="79">
+      <c r="C45" s="128"/>
+      <c r="D45" s="128"/>
+      <c r="E45" s="128"/>
+      <c r="F45" s="128"/>
+      <c r="G45" s="128"/>
+      <c r="H45" s="128"/>
+      <c r="I45" s="128"/>
+      <c r="J45" s="128"/>
+      <c r="K45" s="129"/>
+      <c r="L45" s="22"/>
+      <c r="M45" s="171" t="s">
+        <v>36</v>
+      </c>
+      <c r="N45" s="177" t="s">
+        <v>37</v>
+      </c>
+      <c r="O45" s="175" t="s">
+        <v>63</v>
+      </c>
+      <c r="P45" s="173" t="s">
+        <v>35</v>
+      </c>
+      <c r="T45" s="22"/>
+    </row>
+    <row r="46" spans="2:20" ht="15" customHeight="1">
+      <c r="B46" s="101">
+        <v>1</v>
+      </c>
+      <c r="C46" s="119" t="s">
+        <v>42</v>
+      </c>
+      <c r="D46" s="120"/>
+      <c r="E46" s="120"/>
+      <c r="F46" s="120"/>
+      <c r="G46" s="120"/>
+      <c r="H46" s="120"/>
+      <c r="I46" s="120"/>
+      <c r="J46" s="120"/>
+      <c r="K46" s="121"/>
+      <c r="L46" s="22"/>
+      <c r="M46" s="172"/>
+      <c r="N46" s="178"/>
+      <c r="O46" s="176"/>
+      <c r="P46" s="174"/>
+      <c r="Q46" s="22"/>
+      <c r="R46" s="22"/>
+      <c r="S46" s="22"/>
+      <c r="T46" s="22"/>
+    </row>
+    <row r="47" spans="2:20" ht="15" customHeight="1" thickBot="1">
+      <c r="B47" s="101">
         <f>B46+1</f>
         <v>2</v>
       </c>
-      <c r="C47" s="97" t="s">
-        <v>28</v>
-      </c>
-      <c r="D47" s="98"/>
-      <c r="E47" s="98"/>
-      <c r="F47" s="98"/>
-      <c r="G47" s="98"/>
-      <c r="H47" s="98"/>
-      <c r="I47" s="98"/>
-      <c r="J47" s="98"/>
-      <c r="K47" s="99"/>
-    </row>
-    <row r="48" spans="2:11" ht="15" customHeight="1">
-      <c r="B48" s="79">
+      <c r="C47" s="119" t="s">
+        <v>43</v>
+      </c>
+      <c r="D47" s="120"/>
+      <c r="E47" s="120"/>
+      <c r="F47" s="120"/>
+      <c r="G47" s="120"/>
+      <c r="H47" s="120"/>
+      <c r="I47" s="120"/>
+      <c r="J47" s="120"/>
+      <c r="K47" s="121"/>
+      <c r="L47" s="22"/>
+      <c r="M47" s="150">
+        <f>Q38+Q39+Q40+Q41</f>
+        <v>640</v>
+      </c>
+      <c r="N47" s="151">
+        <f>J37</f>
+        <v>2753.15</v>
+      </c>
+      <c r="O47" s="31">
+        <f>N47-M47</f>
+        <v>2113.15</v>
+      </c>
+      <c r="P47" s="32">
+        <f>O47/N47</f>
+        <v>0.76753900078092363</v>
+      </c>
+      <c r="Q47" s="22"/>
+      <c r="R47" s="22"/>
+      <c r="S47" s="22"/>
+      <c r="T47" s="22"/>
+    </row>
+    <row r="48" spans="2:20" ht="15" customHeight="1">
+      <c r="B48" s="101">
         <f>B47+1</f>
         <v>3</v>
       </c>
-      <c r="C48" s="97" t="s">
-        <v>29</v>
-      </c>
-      <c r="D48" s="98"/>
-      <c r="E48" s="98"/>
-      <c r="F48" s="98"/>
-      <c r="G48" s="98"/>
-      <c r="H48" s="98"/>
-      <c r="I48" s="98"/>
-      <c r="J48" s="98"/>
-      <c r="K48" s="99"/>
-    </row>
-    <row r="49" spans="2:11" ht="15" customHeight="1">
-      <c r="B49" s="79">
-        <f t="shared" ref="B49:B55" si="16">B48+1</f>
+      <c r="C48" s="119" t="s">
+        <v>44</v>
+      </c>
+      <c r="D48" s="120"/>
+      <c r="E48" s="120"/>
+      <c r="F48" s="120"/>
+      <c r="G48" s="120"/>
+      <c r="H48" s="120"/>
+      <c r="I48" s="120"/>
+      <c r="J48" s="120"/>
+      <c r="K48" s="121"/>
+      <c r="L48" s="22"/>
+      <c r="Q48" s="22"/>
+      <c r="R48" s="22"/>
+      <c r="S48" s="22"/>
+      <c r="T48" s="22"/>
+    </row>
+    <row r="49" spans="2:20" ht="15" customHeight="1">
+      <c r="B49" s="101">
+        <f t="shared" ref="B49:B55" si="20">B48+1</f>
         <v>4</v>
       </c>
-      <c r="C49" s="97" t="s">
-        <v>30</v>
-      </c>
-      <c r="D49" s="98"/>
-      <c r="E49" s="98"/>
-      <c r="F49" s="98"/>
-      <c r="G49" s="98"/>
-      <c r="H49" s="98"/>
-      <c r="I49" s="98"/>
-      <c r="J49" s="98"/>
-      <c r="K49" s="99"/>
-    </row>
-    <row r="50" spans="2:11" ht="15" customHeight="1">
-      <c r="B50" s="79">
-        <f t="shared" si="16"/>
+      <c r="C49" s="119" t="s">
+        <v>45</v>
+      </c>
+      <c r="D49" s="120"/>
+      <c r="E49" s="120"/>
+      <c r="F49" s="120"/>
+      <c r="G49" s="120"/>
+      <c r="H49" s="120"/>
+      <c r="I49" s="120"/>
+      <c r="J49" s="120"/>
+      <c r="K49" s="121"/>
+      <c r="L49" s="22"/>
+      <c r="Q49" s="22"/>
+      <c r="R49" s="22"/>
+      <c r="S49" s="22"/>
+      <c r="T49" s="22"/>
+    </row>
+    <row r="50" spans="2:20" ht="15" customHeight="1">
+      <c r="B50" s="101">
+        <f t="shared" si="20"/>
         <v>5</v>
       </c>
-      <c r="C50" s="97" t="s">
-        <v>31</v>
-      </c>
-      <c r="D50" s="98"/>
-      <c r="E50" s="98"/>
-      <c r="F50" s="98"/>
-      <c r="G50" s="98"/>
-      <c r="H50" s="98"/>
-      <c r="I50" s="98"/>
-      <c r="J50" s="98"/>
-      <c r="K50" s="99"/>
-    </row>
-    <row r="51" spans="2:11" ht="15" customHeight="1">
-      <c r="B51" s="79">
+      <c r="C50" s="119" t="s">
+        <v>46</v>
+      </c>
+      <c r="D50" s="120"/>
+      <c r="E50" s="120"/>
+      <c r="F50" s="120"/>
+      <c r="G50" s="120"/>
+      <c r="H50" s="120"/>
+      <c r="I50" s="120"/>
+      <c r="J50" s="120"/>
+      <c r="K50" s="121"/>
+      <c r="L50" s="22"/>
+      <c r="T50" s="22"/>
+    </row>
+    <row r="51" spans="2:20" ht="15" customHeight="1">
+      <c r="B51" s="101">
         <v>6</v>
       </c>
-      <c r="C51" s="97" t="s">
-        <v>32</v>
-      </c>
-      <c r="D51" s="98"/>
-      <c r="E51" s="98"/>
-      <c r="F51" s="98"/>
-      <c r="G51" s="98"/>
-      <c r="H51" s="98"/>
-      <c r="I51" s="98"/>
-      <c r="J51" s="98"/>
-      <c r="K51" s="99"/>
-    </row>
-    <row r="52" spans="2:11" ht="15" customHeight="1">
-      <c r="B52" s="79">
-        <f t="shared" si="16"/>
+      <c r="C51" s="119" t="s">
+        <v>47</v>
+      </c>
+      <c r="D51" s="120"/>
+      <c r="E51" s="120"/>
+      <c r="F51" s="120"/>
+      <c r="G51" s="120"/>
+      <c r="H51" s="120"/>
+      <c r="I51" s="120"/>
+      <c r="J51" s="120"/>
+      <c r="K51" s="121"/>
+      <c r="L51" s="22"/>
+      <c r="T51" s="22"/>
+    </row>
+    <row r="52" spans="2:20" ht="15" customHeight="1">
+      <c r="B52" s="101">
+        <f t="shared" si="20"/>
         <v>7</v>
       </c>
-      <c r="C52" s="97" t="s">
-        <v>33</v>
-      </c>
-      <c r="D52" s="98"/>
-      <c r="E52" s="98"/>
-      <c r="F52" s="98"/>
-      <c r="G52" s="98"/>
-      <c r="H52" s="98"/>
-      <c r="I52" s="98"/>
-      <c r="J52" s="98"/>
-      <c r="K52" s="99"/>
-    </row>
-    <row r="53" spans="2:11" ht="15" customHeight="1">
-      <c r="B53" s="79">
-        <f t="shared" si="16"/>
+      <c r="C52" s="119" t="s">
+        <v>48</v>
+      </c>
+      <c r="D52" s="120"/>
+      <c r="E52" s="120"/>
+      <c r="F52" s="120"/>
+      <c r="G52" s="120"/>
+      <c r="H52" s="120"/>
+      <c r="I52" s="120"/>
+      <c r="J52" s="120"/>
+      <c r="K52" s="121"/>
+      <c r="L52" s="22"/>
+      <c r="T52" s="22"/>
+    </row>
+    <row r="53" spans="2:20" ht="15" customHeight="1">
+      <c r="B53" s="101">
+        <f t="shared" si="20"/>
         <v>8</v>
       </c>
-      <c r="C53" s="97" t="s">
-        <v>34</v>
-      </c>
-      <c r="D53" s="98"/>
-      <c r="E53" s="98"/>
-      <c r="F53" s="98"/>
-      <c r="G53" s="98"/>
-      <c r="H53" s="98"/>
-      <c r="I53" s="98"/>
-      <c r="J53" s="98"/>
-      <c r="K53" s="99"/>
-    </row>
-    <row r="54" spans="2:11" ht="15" customHeight="1">
-      <c r="B54" s="79">
-        <f t="shared" si="16"/>
+      <c r="C53" s="119" t="s">
+        <v>49</v>
+      </c>
+      <c r="D53" s="120"/>
+      <c r="E53" s="120"/>
+      <c r="F53" s="120"/>
+      <c r="G53" s="120"/>
+      <c r="H53" s="120"/>
+      <c r="I53" s="120"/>
+      <c r="J53" s="120"/>
+      <c r="K53" s="121"/>
+      <c r="L53" s="22"/>
+      <c r="T53" s="22"/>
+    </row>
+    <row r="54" spans="2:20" ht="15" customHeight="1">
+      <c r="B54" s="101">
+        <f t="shared" si="20"/>
         <v>9</v>
       </c>
-      <c r="C54" s="97" t="s">
-        <v>35</v>
-      </c>
-      <c r="D54" s="98"/>
-      <c r="E54" s="98"/>
-      <c r="F54" s="98"/>
-      <c r="G54" s="98"/>
-      <c r="H54" s="98"/>
-      <c r="I54" s="98"/>
-      <c r="J54" s="98"/>
-      <c r="K54" s="99"/>
-    </row>
-    <row r="55" spans="2:11" ht="15" customHeight="1">
-      <c r="B55" s="79">
-        <f t="shared" si="16"/>
+      <c r="C54" s="119" t="s">
+        <v>50</v>
+      </c>
+      <c r="D54" s="120"/>
+      <c r="E54" s="120"/>
+      <c r="F54" s="120"/>
+      <c r="G54" s="120"/>
+      <c r="H54" s="120"/>
+      <c r="I54" s="120"/>
+      <c r="J54" s="120"/>
+      <c r="K54" s="121"/>
+      <c r="L54" s="22"/>
+      <c r="T54" s="22"/>
+    </row>
+    <row r="55" spans="2:20" ht="15" customHeight="1">
+      <c r="B55" s="101">
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
-      <c r="C55" s="126" t="s">
-        <v>51</v>
-      </c>
-      <c r="D55" s="127"/>
-      <c r="E55" s="127"/>
-      <c r="F55" s="127"/>
-      <c r="G55" s="127"/>
-      <c r="H55" s="127"/>
-      <c r="I55" s="127"/>
-      <c r="J55" s="127"/>
-      <c r="K55" s="128"/>
-    </row>
-    <row r="56" spans="2:11" ht="15" thickBot="1">
-      <c r="B56" s="57"/>
-      <c r="C56" s="18"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="18"/>
-      <c r="G56" s="18"/>
-      <c r="H56" s="18"/>
-      <c r="I56" s="18"/>
-      <c r="J56" s="18"/>
-      <c r="K56" s="100"/>
-    </row>
-    <row r="57" spans="2:11" ht="20.100000000000001" customHeight="1">
-      <c r="B57" s="107" t="s">
-        <v>39</v>
-      </c>
-      <c r="C57" s="108"/>
-      <c r="D57" s="108"/>
-      <c r="E57" s="108"/>
-      <c r="F57" s="108"/>
-      <c r="G57" s="108"/>
-      <c r="H57" s="108"/>
-      <c r="I57" s="108"/>
-      <c r="J57" s="108"/>
-      <c r="K57" s="109"/>
-    </row>
-    <row r="58" spans="2:11" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B58" s="110"/>
-      <c r="C58" s="111" t="s">
-        <v>52</v>
-      </c>
-      <c r="D58" s="112"/>
-      <c r="E58" s="112"/>
-      <c r="F58" s="112"/>
-      <c r="G58" s="112"/>
-      <c r="H58" s="112"/>
-      <c r="I58" s="112"/>
-      <c r="J58" s="113" t="s">
-        <v>42</v>
-      </c>
-      <c r="K58" s="114">
+      <c r="C55" s="159" t="s">
+        <v>80</v>
+      </c>
+      <c r="D55" s="160"/>
+      <c r="E55" s="160"/>
+      <c r="F55" s="160"/>
+      <c r="G55" s="160"/>
+      <c r="H55" s="160"/>
+      <c r="I55" s="160"/>
+      <c r="J55" s="160"/>
+      <c r="K55" s="161"/>
+      <c r="L55" s="22"/>
+      <c r="T55" s="22"/>
+    </row>
+    <row r="56" spans="2:20" ht="15" thickBot="1">
+      <c r="B56" s="79"/>
+      <c r="C56" s="37"/>
+      <c r="D56" s="37"/>
+      <c r="E56" s="37"/>
+      <c r="F56" s="37"/>
+      <c r="G56" s="37"/>
+      <c r="H56" s="37"/>
+      <c r="I56" s="37"/>
+      <c r="J56" s="37"/>
+      <c r="K56" s="122"/>
+      <c r="L56" s="22"/>
+      <c r="T56" s="22"/>
+    </row>
+    <row r="57" spans="2:20" ht="20.149999999999999" customHeight="1">
+      <c r="B57" s="130" t="s">
+        <v>64</v>
+      </c>
+      <c r="C57" s="131"/>
+      <c r="D57" s="131"/>
+      <c r="E57" s="131"/>
+      <c r="F57" s="131"/>
+      <c r="G57" s="131"/>
+      <c r="H57" s="131"/>
+      <c r="I57" s="131"/>
+      <c r="J57" s="131"/>
+      <c r="K57" s="132"/>
+      <c r="L57" s="22"/>
+      <c r="M57" s="22"/>
+      <c r="N57" s="22"/>
+      <c r="O57" s="22"/>
+      <c r="P57" s="22"/>
+      <c r="Q57" s="22"/>
+      <c r="R57" s="22"/>
+      <c r="S57" s="22"/>
+      <c r="T57" s="22"/>
+    </row>
+    <row r="58" spans="2:20" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="B58" s="133"/>
+      <c r="C58" s="134" t="s">
+        <v>82</v>
+      </c>
+      <c r="D58" s="135"/>
+      <c r="E58" s="135"/>
+      <c r="F58" s="135"/>
+      <c r="G58" s="135"/>
+      <c r="H58" s="135"/>
+      <c r="I58" s="135"/>
+      <c r="J58" s="136" t="s">
+        <v>68</v>
+      </c>
+      <c r="K58" s="137">
         <f ca="1">TODAY()</f>
-        <v>45862</v>
-      </c>
-    </row>
-    <row r="59" spans="2:11">
-      <c r="B59" s="58"/>
-      <c r="K59" s="59"/>
-    </row>
-    <row r="60" spans="2:11" ht="20.399999999999999">
-      <c r="B60" s="147"/>
-      <c r="C60" s="148"/>
-      <c r="D60" s="148"/>
-      <c r="E60" s="148"/>
-      <c r="F60" s="148"/>
-      <c r="G60" s="148"/>
-      <c r="H60" s="148"/>
-      <c r="I60" s="148"/>
-      <c r="J60" s="148"/>
-      <c r="K60" s="149"/>
-    </row>
-    <row r="61" spans="2:11">
-      <c r="B61" s="58"/>
-      <c r="K61" s="59"/>
-    </row>
-    <row r="62" spans="2:11">
-      <c r="B62" s="58"/>
-      <c r="K62" s="59"/>
-    </row>
-    <row r="63" spans="2:11">
-      <c r="B63" s="58"/>
-      <c r="K63" s="59"/>
-    </row>
-    <row r="64" spans="2:11">
-      <c r="B64" s="58"/>
-      <c r="K64" s="59"/>
+        <v>45728</v>
+      </c>
+      <c r="L58" s="22"/>
+      <c r="M58" s="123"/>
+      <c r="N58" s="22"/>
+      <c r="O58" s="22"/>
+      <c r="P58" s="22"/>
+      <c r="Q58" s="22"/>
+      <c r="R58" s="22"/>
+      <c r="S58" s="22"/>
+      <c r="T58" s="22"/>
+    </row>
+    <row r="59" spans="2:20">
+      <c r="B59" s="80"/>
+      <c r="K59" s="81"/>
+    </row>
+    <row r="60" spans="2:20" ht="19.75">
+      <c r="B60" s="168"/>
+      <c r="C60" s="169"/>
+      <c r="D60" s="169"/>
+      <c r="E60" s="169"/>
+      <c r="F60" s="169"/>
+      <c r="G60" s="169"/>
+      <c r="H60" s="169"/>
+      <c r="I60" s="169"/>
+      <c r="J60" s="169"/>
+      <c r="K60" s="170"/>
+    </row>
+    <row r="61" spans="2:20">
+      <c r="B61" s="80"/>
+      <c r="K61" s="81"/>
+    </row>
+    <row r="62" spans="2:20">
+      <c r="B62" s="80"/>
+      <c r="K62" s="81"/>
+    </row>
+    <row r="63" spans="2:20">
+      <c r="B63" s="80"/>
+      <c r="K63" s="81"/>
+    </row>
+    <row r="64" spans="2:20">
+      <c r="B64" s="80"/>
+      <c r="K64" s="81"/>
     </row>
     <row r="65" spans="2:11">
-      <c r="B65" s="58"/>
-      <c r="K65" s="59"/>
+      <c r="B65" s="80"/>
+      <c r="K65" s="81"/>
     </row>
     <row r="66" spans="2:11">
-      <c r="B66" s="58"/>
-      <c r="K66" s="59"/>
+      <c r="B66" s="80"/>
+      <c r="K66" s="81"/>
     </row>
     <row r="67" spans="2:11">
-      <c r="B67" s="58"/>
-      <c r="K67" s="59"/>
+      <c r="B67" s="80"/>
+      <c r="K67" s="81"/>
     </row>
     <row r="68" spans="2:11" ht="15" thickBot="1">
-      <c r="B68" s="60"/>
-      <c r="C68" s="61"/>
-      <c r="D68" s="61"/>
-      <c r="E68" s="61"/>
-      <c r="F68" s="61"/>
-      <c r="G68" s="61"/>
-      <c r="H68" s="61"/>
-      <c r="I68" s="61"/>
-      <c r="J68" s="61"/>
-      <c r="K68" s="62"/>
+      <c r="B68" s="82"/>
+      <c r="C68" s="83"/>
+      <c r="D68" s="83"/>
+      <c r="E68" s="83"/>
+      <c r="F68" s="83"/>
+      <c r="G68" s="83"/>
+      <c r="H68" s="83"/>
+      <c r="I68" s="83"/>
+      <c r="J68" s="83"/>
+      <c r="K68" s="84"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B60:K60"/>
+  <mergeCells count="14">
+    <mergeCell ref="N42:N43"/>
+    <mergeCell ref="N36:Q36"/>
     <mergeCell ref="D3:G4"/>
     <mergeCell ref="B6:K8"/>
+    <mergeCell ref="M42:M43"/>
+    <mergeCell ref="O42:O43"/>
+    <mergeCell ref="P42:P43"/>
     <mergeCell ref="B9:K9"/>
     <mergeCell ref="B10:K10"/>
+    <mergeCell ref="B60:K60"/>
+    <mergeCell ref="M45:M46"/>
+    <mergeCell ref="P45:P46"/>
+    <mergeCell ref="O45:O46"/>
+    <mergeCell ref="N45:N46"/>
   </mergeCells>
   <phoneticPr fontId="36" type="noConversion"/>
+  <conditionalFormatting sqref="R15:R17">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",R15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",R15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R21:R24">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",R21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",R21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.1" bottom="0.75" header="0.5" footer="0.3"/>
   <pageSetup paperSize="9" scale="44" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Integrate doprava data export to Excel report
Added export of transportation (doprava) data to the Excel report by introducing load_doprava_data and save_doprava_data functions in doprava.py. Updated excel_processing.py to append doprava data to the generated Excel file. Improved code structure and UI in doprava.py for better clarity and user experience.
</commit_message>
<xml_diff>
--- a/one folder to rule them all/Hlavna aplikacia/CPINT.xlsx
+++ b/one folder to rule them all/Hlavna aplikacia/CPINT.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="Tento_zošit"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slaso\Documents\GitHub\one folder to rule them all\Hlavna aplikacia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\LastMile\one folder to rule them all\Hlavna aplikacia\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACCFD28-3A97-4B5B-BD1E-460EB5B26DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="33120" windowHeight="18000"/>
+    <workbookView xWindow="8460" yWindow="1425" windowWidth="28800" windowHeight="18765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CP" sheetId="30" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <definedName name="AND">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">CP!$B$2:$K$37</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>PČ</t>
   </si>
@@ -87,18 +88,6 @@
   </si>
   <si>
     <t>Plat €/h</t>
-  </si>
-  <si>
-    <t>Projektant</t>
-  </si>
-  <si>
-    <t>SLP technik</t>
-  </si>
-  <si>
-    <t>Stavbyvedúci</t>
-  </si>
-  <si>
-    <t>IP technik</t>
   </si>
   <si>
     <t>Nákup materiál SPOLU</t>
@@ -221,7 +210,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
     <numFmt numFmtId="164" formatCode="#,##0.00&quot; Sk&quot;"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ _S_k"/>
@@ -1533,7 +1522,7 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1813,17 +1802,14 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="35" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="35" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="26" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="26" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1837,12 +1823,39 @@
     <xf numFmtId="0" fontId="27" fillId="26" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="48" fillId="21" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="21" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="48" fillId="21" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="48" fillId="21" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="48" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="23" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="33" xfId="59" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="59" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="34" xfId="59" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="37" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1870,24 +1883,6 @@
     <xf numFmtId="0" fontId="51" fillId="30" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="21" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="21" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="23" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="49" fillId="30" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1906,96 +1901,84 @@
     <xf numFmtId="0" fontId="50" fillId="30" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="33" xfId="59" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="59" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="34" xfId="59" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="61">
-    <cellStyle name="20 % - zvýraznenie1 2" xfId="16"/>
-    <cellStyle name="20 % - zvýraznenie2 2" xfId="17"/>
-    <cellStyle name="20 % - zvýraznenie3 2" xfId="18"/>
-    <cellStyle name="20 % - zvýraznenie4 2" xfId="19"/>
-    <cellStyle name="20 % - zvýraznenie5 2" xfId="20"/>
-    <cellStyle name="20 % - zvýraznenie6 2" xfId="21"/>
-    <cellStyle name="40 % - zvýraznenie1 2" xfId="22"/>
-    <cellStyle name="40 % - zvýraznenie2 2" xfId="23"/>
-    <cellStyle name="40 % - zvýraznenie3 2" xfId="24"/>
-    <cellStyle name="40 % - zvýraznenie4 2" xfId="25"/>
-    <cellStyle name="40 % - zvýraznenie5 2" xfId="26"/>
-    <cellStyle name="40 % - zvýraznenie6 2" xfId="27"/>
-    <cellStyle name="60 % - zvýraznenie1 2" xfId="28"/>
-    <cellStyle name="60 % - zvýraznenie2 2" xfId="29"/>
-    <cellStyle name="60 % - zvýraznenie3 2" xfId="30"/>
-    <cellStyle name="60 % - zvýraznenie4 2" xfId="31"/>
-    <cellStyle name="60 % - zvýraznenie5 2" xfId="32"/>
-    <cellStyle name="60 % - zvýraznenie6 2" xfId="33"/>
-    <cellStyle name="čiarky 2" xfId="7"/>
-    <cellStyle name="Dobrá 2" xfId="34"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8"/>
-    <cellStyle name="Hypertextové prepojenie 2" xfId="5"/>
-    <cellStyle name="Kontrolná bunka 2" xfId="35"/>
-    <cellStyle name="lehký dolní okraj" xfId="36"/>
-    <cellStyle name="Mena 2" xfId="37"/>
-    <cellStyle name="nadpis" xfId="38"/>
-    <cellStyle name="Nadpis 1 2" xfId="39"/>
-    <cellStyle name="Nadpis 2 2" xfId="40"/>
-    <cellStyle name="Nadpis 3 2" xfId="41"/>
-    <cellStyle name="Nadpis 4 2" xfId="42"/>
-    <cellStyle name="Neutrálna 2" xfId="43"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="8"/>
-    <cellStyle name="Normálna 2" xfId="2"/>
-    <cellStyle name="Normálna 2 2" xfId="14"/>
-    <cellStyle name="Normálna 3" xfId="15"/>
-    <cellStyle name="Normálna 4" xfId="60"/>
-    <cellStyle name="Normálna 6" xfId="12"/>
-    <cellStyle name="Normálna 7" xfId="13"/>
-    <cellStyle name="Normálne 2" xfId="1"/>
-    <cellStyle name="normálne 2 2" xfId="9"/>
-    <cellStyle name="Normálne 3" xfId="3"/>
-    <cellStyle name="Normálne 4" xfId="10"/>
-    <cellStyle name="Normálne 5" xfId="11"/>
-    <cellStyle name="normální 2" xfId="4"/>
-    <cellStyle name="normální_POL.XLS" xfId="6"/>
-    <cellStyle name="Poznámka 2" xfId="44"/>
-    <cellStyle name="Prepojená bunka 2" xfId="45"/>
-    <cellStyle name="Spolu 2" xfId="46"/>
-    <cellStyle name="Text upozornenia 2" xfId="47"/>
-    <cellStyle name="Vstup 2" xfId="48"/>
-    <cellStyle name="Výpočet 2" xfId="49"/>
-    <cellStyle name="Výstup 2" xfId="50"/>
-    <cellStyle name="Vysvetľujúci text 2" xfId="51"/>
-    <cellStyle name="Zlá 2" xfId="52"/>
-    <cellStyle name="Zvýraznenie1 2" xfId="53"/>
-    <cellStyle name="Zvýraznenie2 2" xfId="54"/>
-    <cellStyle name="Zvýraznenie3 2" xfId="55"/>
-    <cellStyle name="Zvýraznenie4 2" xfId="56"/>
-    <cellStyle name="Zvýraznenie5 2" xfId="57"/>
-    <cellStyle name="Zvýraznenie6 2" xfId="58"/>
+    <cellStyle name="20 % - zvýraznenie1 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="20 % - zvýraznenie2 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="20 % - zvýraznenie3 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="20 % - zvýraznenie4 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="20 % - zvýraznenie5 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="20 % - zvýraznenie6 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="40 % - zvýraznenie1 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="40 % - zvýraznenie2 2" xfId="23" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="40 % - zvýraznenie3 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="40 % - zvýraznenie4 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="40 % - zvýraznenie5 2" xfId="26" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="40 % - zvýraznenie6 2" xfId="27" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="60 % - zvýraznenie1 2" xfId="28" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="60 % - zvýraznenie2 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="60 % - zvýraznenie3 2" xfId="30" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="60 % - zvýraznenie4 2" xfId="31" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="60 % - zvýraznenie5 2" xfId="32" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="60 % - zvýraznenie6 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="čiarky 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Dobrá 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Hypertextové prepojenie" xfId="59" builtinId="8"/>
+    <cellStyle name="Hypertextové prepojenie 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Kontrolná bunka 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="lehký dolní okraj" xfId="36" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Mena 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="nadpis" xfId="38" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Nadpis 1 2" xfId="39" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Nadpis 2 2" xfId="40" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Nadpis 3 2" xfId="41" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Nadpis 4 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Neutrálna 2" xfId="43" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Normal 3" xfId="8" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
+    <cellStyle name="Normálna 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Normálna 2 2" xfId="14" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Normálna 3" xfId="15" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Normálna 4" xfId="60" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Normálna 6" xfId="12" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Normálna 7" xfId="13" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Normálne 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="normálne 2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Normálne 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Normálne 4" xfId="10" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Normálne 5" xfId="11" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="normální 2" xfId="4" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="normální_POL.XLS" xfId="6" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Poznámka 2" xfId="44" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Prepojená bunka 2" xfId="45" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Spolu 2" xfId="46" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Text upozornenia 2" xfId="47" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Vstup 2" xfId="48" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Výpočet 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Výstup 2" xfId="50" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Vysvetľujúci text 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Zlá 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="Zvýraznenie1 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="Zvýraznenie2 2" xfId="54" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="Zvýraznenie3 2" xfId="55" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Zvýraznenie4 2" xfId="56" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="Zvýraznenie5 2" xfId="57" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="Zvýraznenie6 2" xfId="58" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2044,7 +2027,7 @@
         <xdr:cNvPr id="14" name="Obrázok 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DB7B07B5-FAE2-FB54-2448-E1CCD3E523B6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB7B07B5-FAE2-FB54-2448-E1CCD3E523B6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2095,7 +2078,7 @@
         <xdr:cNvPr id="5" name="Obrázok 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{94490EEA-3500-4A23-96AC-19B01E18C0FE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94490EEA-3500-4A23-96AC-19B01E18C0FE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2144,7 +2127,7 @@
         <xdr:cNvPr id="4" name="Obrázok 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3F91FD3D-CBAA-C8DC-12EB-C06FEB5CD61F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F91FD3D-CBAA-C8DC-12EB-C06FEB5CD61F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2440,7 +2423,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hárok1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2448,7 +2431,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
+      <selection pane="bottomLeft" activeCell="M22" sqref="M22:Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2494,10 +2477,10 @@
       <c r="A3" s="1"/>
       <c r="B3" s="26"/>
       <c r="C3" s="27"/>
-      <c r="D3" s="121"/>
-      <c r="E3" s="121"/>
-      <c r="F3" s="121"/>
-      <c r="G3" s="121"/>
+      <c r="D3" s="129"/>
+      <c r="E3" s="129"/>
+      <c r="F3" s="129"/>
+      <c r="G3" s="129"/>
       <c r="H3" s="28"/>
       <c r="I3" s="28"/>
       <c r="J3" s="28"/>
@@ -2507,10 +2490,10 @@
       <c r="A4" s="1"/>
       <c r="B4" s="26"/>
       <c r="C4" s="27"/>
-      <c r="D4" s="121"/>
-      <c r="E4" s="121"/>
-      <c r="F4" s="121"/>
-      <c r="G4" s="121"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="129"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="129"/>
       <c r="H4" s="28"/>
       <c r="I4" s="28"/>
       <c r="J4" s="28"/>
@@ -2531,73 +2514,73 @@
     </row>
     <row r="6" spans="1:20" outlineLevel="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="122" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="123"/>
-      <c r="G6" s="123"/>
-      <c r="H6" s="123"/>
-      <c r="I6" s="123"/>
-      <c r="J6" s="123"/>
-      <c r="K6" s="124"/>
+      <c r="B6" s="130" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="131"/>
+      <c r="D6" s="131"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="131"/>
+      <c r="G6" s="131"/>
+      <c r="H6" s="131"/>
+      <c r="I6" s="131"/>
+      <c r="J6" s="131"/>
+      <c r="K6" s="132"/>
     </row>
     <row r="7" spans="1:20" outlineLevel="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="125"/>
-      <c r="C7" s="126"/>
-      <c r="D7" s="126"/>
-      <c r="E7" s="126"/>
-      <c r="F7" s="126"/>
-      <c r="G7" s="126"/>
-      <c r="H7" s="126"/>
-      <c r="I7" s="126"/>
-      <c r="J7" s="126"/>
-      <c r="K7" s="127"/>
+      <c r="B7" s="133"/>
+      <c r="C7" s="134"/>
+      <c r="D7" s="134"/>
+      <c r="E7" s="134"/>
+      <c r="F7" s="134"/>
+      <c r="G7" s="134"/>
+      <c r="H7" s="134"/>
+      <c r="I7" s="134"/>
+      <c r="J7" s="134"/>
+      <c r="K7" s="135"/>
     </row>
     <row r="8" spans="1:20" outlineLevel="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="125"/>
-      <c r="C8" s="126"/>
-      <c r="D8" s="126"/>
-      <c r="E8" s="126"/>
-      <c r="F8" s="126"/>
-      <c r="G8" s="126"/>
-      <c r="H8" s="126"/>
-      <c r="I8" s="126"/>
-      <c r="J8" s="126"/>
-      <c r="K8" s="127"/>
+      <c r="B8" s="133"/>
+      <c r="C8" s="134"/>
+      <c r="D8" s="134"/>
+      <c r="E8" s="134"/>
+      <c r="F8" s="134"/>
+      <c r="G8" s="134"/>
+      <c r="H8" s="134"/>
+      <c r="I8" s="134"/>
+      <c r="J8" s="134"/>
+      <c r="K8" s="135"/>
     </row>
     <row r="9" spans="1:20" ht="31.5" customHeight="1" outlineLevel="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="134" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="135"/>
-      <c r="D9" s="135"/>
-      <c r="E9" s="135"/>
-      <c r="F9" s="135"/>
-      <c r="G9" s="135"/>
-      <c r="H9" s="135"/>
-      <c r="I9" s="135"/>
-      <c r="J9" s="135"/>
-      <c r="K9" s="136"/>
+      <c r="B9" s="136" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="137"/>
+      <c r="D9" s="137"/>
+      <c r="E9" s="137"/>
+      <c r="F9" s="137"/>
+      <c r="G9" s="137"/>
+      <c r="H9" s="137"/>
+      <c r="I9" s="137"/>
+      <c r="J9" s="137"/>
+      <c r="K9" s="138"/>
     </row>
     <row r="10" spans="1:20" ht="19.7" customHeight="1" outlineLevel="1" thickBot="1">
-      <c r="B10" s="137" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="138"/>
-      <c r="D10" s="138"/>
-      <c r="E10" s="138"/>
-      <c r="F10" s="138"/>
-      <c r="G10" s="138"/>
-      <c r="H10" s="138"/>
-      <c r="I10" s="138"/>
-      <c r="J10" s="138"/>
-      <c r="K10" s="139"/>
+      <c r="B10" s="139" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="140"/>
+      <c r="D10" s="140"/>
+      <c r="E10" s="140"/>
+      <c r="F10" s="140"/>
+      <c r="G10" s="140"/>
+      <c r="H10" s="140"/>
+      <c r="I10" s="140"/>
+      <c r="J10" s="140"/>
+      <c r="K10" s="141"/>
     </row>
     <row r="11" spans="1:20" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="A11" s="2"/>
@@ -2646,25 +2629,25 @@
       </c>
       <c r="L12" s="12"/>
       <c r="M12" s="99" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="N12" s="99" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="O12" s="99" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="P12" s="99" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="Q12" s="100" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="R12" s="99" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="S12" s="100" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="9.9499999999999993" customHeight="1">
@@ -2705,7 +2688,7 @@
       <c r="N14" s="9"/>
       <c r="O14" s="9"/>
       <c r="P14" s="18"/>
-      <c r="Q14" s="112"/>
+      <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
       <c r="S14" s="9"/>
       <c r="T14" s="9"/>
@@ -2730,7 +2713,7 @@
       <c r="D16" s="63"/>
       <c r="E16" s="64"/>
       <c r="F16" s="54" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G16" s="55" t="e">
         <f>#REF!+#REF!+#REF!</f>
@@ -2738,7 +2721,7 @@
       </c>
       <c r="H16" s="74"/>
       <c r="I16" s="54" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J16" s="55" t="e">
         <f>#REF!+#REF!+#REF!</f>
@@ -2821,18 +2804,18 @@
         <v>#REF!</v>
       </c>
       <c r="L20" s="9"/>
-      <c r="M20" s="143" t="s">
-        <v>42</v>
-      </c>
-      <c r="N20" s="145" t="s">
-        <v>40</v>
-      </c>
-      <c r="O20" s="145" t="s">
-        <v>41</v>
-      </c>
-      <c r="P20" s="148"/>
-      <c r="Q20" s="147" t="s">
-        <v>43</v>
+      <c r="M20" s="142" t="s">
+        <v>38</v>
+      </c>
+      <c r="N20" s="144" t="s">
+        <v>36</v>
+      </c>
+      <c r="O20" s="144" t="s">
+        <v>37</v>
+      </c>
+      <c r="P20" s="146"/>
+      <c r="Q20" s="142" t="s">
+        <v>39</v>
       </c>
       <c r="T20" s="9"/>
     </row>
@@ -2854,11 +2837,11 @@
         <v>#REF!</v>
       </c>
       <c r="L21" s="9"/>
-      <c r="M21" s="144"/>
-      <c r="N21" s="146"/>
-      <c r="O21" s="146"/>
-      <c r="P21" s="148"/>
-      <c r="Q21" s="147"/>
+      <c r="M21" s="143"/>
+      <c r="N21" s="145"/>
+      <c r="O21" s="145"/>
+      <c r="P21" s="146"/>
+      <c r="Q21" s="142"/>
       <c r="R21" s="11"/>
       <c r="T21" s="9"/>
     </row>
@@ -2872,27 +2855,18 @@
       <c r="H22" s="63"/>
       <c r="I22" s="62"/>
       <c r="J22" s="96" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="K22" s="65" t="e">
         <f>SUM(K19:K21)</f>
         <v>#REF!</v>
       </c>
       <c r="L22" s="9"/>
-      <c r="M22" s="10">
-        <v>10</v>
-      </c>
-      <c r="N22" s="10">
-        <v>1</v>
-      </c>
-      <c r="O22" s="10">
-        <f>M22*N22</f>
-        <v>10</v>
-      </c>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
       <c r="P22" s="9"/>
-      <c r="Q22" s="12">
-        <v>0.1</v>
-      </c>
+      <c r="Q22" s="12"/>
       <c r="R22" s="12"/>
       <c r="T22" s="9"/>
     </row>
@@ -2931,12 +2905,12 @@
       <c r="K24" s="79"/>
       <c r="L24" s="9"/>
       <c r="M24" s="13"/>
-      <c r="N24" s="119" t="s">
+      <c r="N24" s="127" t="s">
         <v>12</v>
       </c>
-      <c r="O24" s="120"/>
-      <c r="P24" s="120"/>
-      <c r="Q24" s="120"/>
+      <c r="O24" s="128"/>
+      <c r="P24" s="128"/>
+      <c r="Q24" s="128"/>
       <c r="R24" s="13"/>
       <c r="T24" s="9"/>
     </row>
@@ -2945,7 +2919,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="69" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D25" s="70"/>
       <c r="E25" s="70"/>
@@ -2970,7 +2944,7 @@
         <v>4</v>
       </c>
       <c r="R25" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="S25" s="9"/>
       <c r="T25" s="9"/>
@@ -2981,7 +2955,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="69" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D26" s="70"/>
       <c r="E26" s="70"/>
@@ -2992,26 +2966,12 @@
       <c r="J26" s="70"/>
       <c r="K26" s="71"/>
       <c r="L26" s="9"/>
-      <c r="M26" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N26" s="101">
-        <v>1</v>
-      </c>
-      <c r="O26" s="102">
-        <v>8</v>
-      </c>
-      <c r="P26" s="103">
-        <v>5</v>
-      </c>
-      <c r="Q26" s="103">
-        <f>N26*(O26*P26)</f>
-        <v>40</v>
-      </c>
-      <c r="R26" s="8">
-        <f>Q26*1.1</f>
-        <v>44</v>
-      </c>
+      <c r="M26" s="5"/>
+      <c r="N26" s="101"/>
+      <c r="O26" s="102"/>
+      <c r="P26" s="103"/>
+      <c r="Q26" s="103"/>
+      <c r="R26" s="8"/>
       <c r="S26" s="9"/>
       <c r="T26" s="9"/>
     </row>
@@ -3021,7 +2981,7 @@
         <v>3</v>
       </c>
       <c r="C27" s="69" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D27" s="70"/>
       <c r="E27" s="70"/>
@@ -3031,26 +2991,12 @@
       <c r="I27" s="70"/>
       <c r="J27" s="70"/>
       <c r="K27" s="71"/>
-      <c r="M27" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="N27" s="101">
-        <v>2</v>
-      </c>
-      <c r="O27" s="102">
-        <v>16</v>
-      </c>
-      <c r="P27" s="103">
-        <v>10</v>
-      </c>
-      <c r="Q27" s="103">
-        <f>N27*(O27*P27)</f>
-        <v>320</v>
-      </c>
-      <c r="R27" s="8">
-        <f>Q27*1.1</f>
-        <v>352</v>
-      </c>
+      <c r="M27" s="5"/>
+      <c r="N27" s="101"/>
+      <c r="O27" s="102"/>
+      <c r="P27" s="103"/>
+      <c r="Q27" s="103"/>
+      <c r="R27" s="8"/>
       <c r="S27" s="9"/>
       <c r="T27" s="9"/>
     </row>
@@ -3060,7 +3006,7 @@
         <v>4</v>
       </c>
       <c r="C28" s="69" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D28" s="70"/>
       <c r="E28" s="70"/>
@@ -3071,26 +3017,12 @@
       <c r="J28" s="70"/>
       <c r="K28" s="71"/>
       <c r="L28" s="9"/>
-      <c r="M28" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N28" s="101">
-        <v>1</v>
-      </c>
-      <c r="O28" s="102">
-        <v>8</v>
-      </c>
-      <c r="P28" s="103">
-        <v>15</v>
-      </c>
-      <c r="Q28" s="103">
-        <f>N28*(O28*P28)</f>
-        <v>120</v>
-      </c>
-      <c r="R28" s="8">
-        <f>Q28*1.1</f>
-        <v>132</v>
-      </c>
+      <c r="M28" s="5"/>
+      <c r="N28" s="101"/>
+      <c r="O28" s="102"/>
+      <c r="P28" s="103"/>
+      <c r="Q28" s="103"/>
+      <c r="R28" s="8"/>
       <c r="S28" s="9"/>
       <c r="T28" s="9"/>
     </row>
@@ -3100,7 +3032,7 @@
         <v>5</v>
       </c>
       <c r="C29" s="69" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D29" s="70"/>
       <c r="E29" s="70"/>
@@ -3111,26 +3043,12 @@
       <c r="J29" s="70"/>
       <c r="K29" s="71"/>
       <c r="L29" s="9"/>
-      <c r="M29" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="N29" s="101">
-        <v>1</v>
-      </c>
-      <c r="O29" s="102">
-        <v>8</v>
-      </c>
-      <c r="P29" s="103">
-        <v>20</v>
-      </c>
-      <c r="Q29" s="103">
-        <f>N29*(O29*P29)</f>
-        <v>160</v>
-      </c>
-      <c r="R29" s="8">
-        <f>Q29*1.1</f>
-        <v>176</v>
-      </c>
+      <c r="M29" s="5"/>
+      <c r="N29" s="101"/>
+      <c r="O29" s="102"/>
+      <c r="P29" s="103"/>
+      <c r="Q29" s="103"/>
+      <c r="R29" s="8"/>
       <c r="T29" s="9"/>
     </row>
     <row r="30" spans="2:20" ht="15" customHeight="1">
@@ -3138,7 +3056,7 @@
         <v>6</v>
       </c>
       <c r="C30" s="69" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D30" s="70"/>
       <c r="E30" s="70"/>
@@ -3149,17 +3067,17 @@
       <c r="J30" s="70"/>
       <c r="K30" s="71"/>
       <c r="L30" s="9"/>
-      <c r="M30" s="128" t="s">
-        <v>20</v>
-      </c>
-      <c r="N30" s="117" t="s">
-        <v>48</v>
-      </c>
-      <c r="O30" s="130" t="s">
+      <c r="M30" s="116" t="s">
+        <v>16</v>
+      </c>
+      <c r="N30" s="118" t="s">
         <v>44</v>
       </c>
-      <c r="P30" s="132" t="s">
-        <v>21</v>
+      <c r="O30" s="120" t="s">
+        <v>40</v>
+      </c>
+      <c r="P30" s="122" t="s">
+        <v>17</v>
       </c>
       <c r="T30" s="9"/>
     </row>
@@ -3169,7 +3087,7 @@
         <v>7</v>
       </c>
       <c r="C31" s="69" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D31" s="70"/>
       <c r="E31" s="70"/>
@@ -3180,10 +3098,10 @@
       <c r="J31" s="70"/>
       <c r="K31" s="71"/>
       <c r="L31" s="9"/>
-      <c r="M31" s="129"/>
-      <c r="N31" s="118"/>
-      <c r="O31" s="131"/>
-      <c r="P31" s="133"/>
+      <c r="M31" s="117"/>
+      <c r="N31" s="119"/>
+      <c r="O31" s="121"/>
+      <c r="P31" s="123"/>
       <c r="T31" s="9"/>
     </row>
     <row r="32" spans="2:20" ht="15" customHeight="1" thickBot="1">
@@ -3192,7 +3110,7 @@
         <v>8</v>
       </c>
       <c r="C32" s="69" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D32" s="70"/>
       <c r="E32" s="70"/>
@@ -3227,7 +3145,7 @@
         <v>9</v>
       </c>
       <c r="C33" s="69" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D33" s="70"/>
       <c r="E33" s="70"/>
@@ -3238,17 +3156,17 @@
       <c r="J33" s="70"/>
       <c r="K33" s="71"/>
       <c r="L33" s="9"/>
-      <c r="M33" s="113" t="s">
-        <v>22</v>
-      </c>
-      <c r="N33" s="115" t="s">
-        <v>23</v>
-      </c>
-      <c r="O33" s="130" t="s">
-        <v>46</v>
-      </c>
-      <c r="P33" s="132" t="s">
-        <v>21</v>
+      <c r="M33" s="112" t="s">
+        <v>18</v>
+      </c>
+      <c r="N33" s="114" t="s">
+        <v>19</v>
+      </c>
+      <c r="O33" s="120" t="s">
+        <v>42</v>
+      </c>
+      <c r="P33" s="122" t="s">
+        <v>17</v>
       </c>
       <c r="T33" s="9"/>
     </row>
@@ -3258,7 +3176,7 @@
         <v>10</v>
       </c>
       <c r="C34" s="105" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D34" s="106"/>
       <c r="E34" s="106"/>
@@ -3269,10 +3187,10 @@
       <c r="J34" s="106"/>
       <c r="K34" s="107"/>
       <c r="L34" s="9"/>
-      <c r="M34" s="114"/>
-      <c r="N34" s="116"/>
-      <c r="O34" s="131"/>
-      <c r="P34" s="133"/>
+      <c r="M34" s="113"/>
+      <c r="N34" s="115"/>
+      <c r="O34" s="121"/>
+      <c r="P34" s="123"/>
       <c r="Q34" s="9"/>
       <c r="R34" s="9"/>
       <c r="T34" s="9"/>
@@ -3291,7 +3209,7 @@
       <c r="L35" s="9"/>
       <c r="M35" s="97">
         <f>Q26+Q27+Q28+Q29</f>
-        <v>640</v>
+        <v>0</v>
       </c>
       <c r="N35" s="98" t="e">
         <f>J16</f>
@@ -3311,7 +3229,7 @@
     </row>
     <row r="36" spans="2:20" ht="20.100000000000001" customHeight="1">
       <c r="B36" s="80" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C36" s="81"/>
       <c r="D36" s="81"/>
@@ -3335,7 +3253,7 @@
     <row r="37" spans="2:20" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="B37" s="83"/>
       <c r="C37" s="84" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D37" s="85"/>
       <c r="E37" s="85"/>
@@ -3344,11 +3262,11 @@
       <c r="H37" s="85"/>
       <c r="I37" s="85"/>
       <c r="J37" s="86" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="K37" s="87">
         <f ca="1">TODAY()</f>
-        <v>45899</v>
+        <v>45918</v>
       </c>
       <c r="L37" s="9"/>
       <c r="M37" s="73"/>
@@ -3365,16 +3283,16 @@
       <c r="K38" s="48"/>
     </row>
     <row r="39" spans="2:20" ht="19.5">
-      <c r="B39" s="140"/>
-      <c r="C39" s="141"/>
-      <c r="D39" s="141"/>
-      <c r="E39" s="141"/>
-      <c r="F39" s="141"/>
-      <c r="G39" s="141"/>
-      <c r="H39" s="141"/>
-      <c r="I39" s="141"/>
-      <c r="J39" s="141"/>
-      <c r="K39" s="142"/>
+      <c r="B39" s="124"/>
+      <c r="C39" s="125"/>
+      <c r="D39" s="125"/>
+      <c r="E39" s="125"/>
+      <c r="F39" s="125"/>
+      <c r="G39" s="125"/>
+      <c r="H39" s="125"/>
+      <c r="I39" s="125"/>
+      <c r="J39" s="125"/>
+      <c r="K39" s="126"/>
     </row>
     <row r="40" spans="2:20" ht="15" customHeight="1">
       <c r="B40" s="47"/>
@@ -3418,12 +3336,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="M30:M31"/>
-    <mergeCell ref="N30:N31"/>
-    <mergeCell ref="O30:O31"/>
-    <mergeCell ref="P30:P31"/>
-    <mergeCell ref="O33:O34"/>
-    <mergeCell ref="P33:P34"/>
     <mergeCell ref="B39:K39"/>
     <mergeCell ref="N24:Q24"/>
     <mergeCell ref="D3:G4"/>
@@ -3435,6 +3347,12 @@
     <mergeCell ref="O20:O21"/>
     <mergeCell ref="Q20:Q21"/>
     <mergeCell ref="P20:P21"/>
+    <mergeCell ref="M30:M31"/>
+    <mergeCell ref="N30:N31"/>
+    <mergeCell ref="O30:O31"/>
+    <mergeCell ref="P30:P31"/>
+    <mergeCell ref="O33:O34"/>
+    <mergeCell ref="P33:P34"/>
   </mergeCells>
   <phoneticPr fontId="34" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Update CPINT.xlsx with latest data
The CPINT.xlsx file has been updated. Changes may include new or modified data, formulas, or formatting.
</commit_message>
<xml_diff>
--- a/one folder to rule them all/Hlavna aplikacia/CPINT.xlsx
+++ b/one folder to rule them all/Hlavna aplikacia/CPINT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\LastMile\one folder to rule them all\Hlavna aplikacia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACCFD28-3A97-4B5B-BD1E-460EB5B26DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68921340-C69F-41D2-95CE-778E55283F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8460" yWindow="1425" windowWidth="28800" windowHeight="18765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5070" yWindow="5070" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CP" sheetId="30" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
   <si>
     <t>PČ</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>xxx, +421 9..., xxx@lastmile.sk</t>
+  </si>
+  <si>
+    <t>Cena za 1 km</t>
   </si>
 </sst>
 </file>
@@ -1823,6 +1826,75 @@
     <xf numFmtId="0" fontId="27" fillId="26" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="33" xfId="59" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="59" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="34" xfId="59" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="30" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="30" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="30" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="30" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="30" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="30" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="30" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="30" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="30" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="30" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="30" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="30" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="48" fillId="21" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1846,75 +1918,6 @@
     </xf>
     <xf numFmtId="0" fontId="48" fillId="23" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="33" xfId="59" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="59" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="34" xfId="59" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="30" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="30" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="30" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="30" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="30" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="30" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="30" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="30" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="30" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="30" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="30" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="30" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="61">
@@ -2431,7 +2434,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M22" sqref="M22:Q22"/>
+      <selection pane="bottomLeft" activeCell="P20" sqref="P20:P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2477,10 +2480,10 @@
       <c r="A3" s="1"/>
       <c r="B3" s="26"/>
       <c r="C3" s="27"/>
-      <c r="D3" s="129"/>
-      <c r="E3" s="129"/>
-      <c r="F3" s="129"/>
-      <c r="G3" s="129"/>
+      <c r="D3" s="121"/>
+      <c r="E3" s="121"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
       <c r="H3" s="28"/>
       <c r="I3" s="28"/>
       <c r="J3" s="28"/>
@@ -2490,10 +2493,10 @@
       <c r="A4" s="1"/>
       <c r="B4" s="26"/>
       <c r="C4" s="27"/>
-      <c r="D4" s="129"/>
-      <c r="E4" s="129"/>
-      <c r="F4" s="129"/>
-      <c r="G4" s="129"/>
+      <c r="D4" s="121"/>
+      <c r="E4" s="121"/>
+      <c r="F4" s="121"/>
+      <c r="G4" s="121"/>
       <c r="H4" s="28"/>
       <c r="I4" s="28"/>
       <c r="J4" s="28"/>
@@ -2514,73 +2517,73 @@
     </row>
     <row r="6" spans="1:20" outlineLevel="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="130" t="s">
+      <c r="B6" s="122" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="131"/>
-      <c r="D6" s="131"/>
-      <c r="E6" s="131"/>
-      <c r="F6" s="131"/>
-      <c r="G6" s="131"/>
-      <c r="H6" s="131"/>
-      <c r="I6" s="131"/>
-      <c r="J6" s="131"/>
-      <c r="K6" s="132"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="123"/>
+      <c r="F6" s="123"/>
+      <c r="G6" s="123"/>
+      <c r="H6" s="123"/>
+      <c r="I6" s="123"/>
+      <c r="J6" s="123"/>
+      <c r="K6" s="124"/>
     </row>
     <row r="7" spans="1:20" outlineLevel="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="133"/>
-      <c r="C7" s="134"/>
-      <c r="D7" s="134"/>
-      <c r="E7" s="134"/>
-      <c r="F7" s="134"/>
-      <c r="G7" s="134"/>
-      <c r="H7" s="134"/>
-      <c r="I7" s="134"/>
-      <c r="J7" s="134"/>
-      <c r="K7" s="135"/>
+      <c r="B7" s="125"/>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="126"/>
+      <c r="F7" s="126"/>
+      <c r="G7" s="126"/>
+      <c r="H7" s="126"/>
+      <c r="I7" s="126"/>
+      <c r="J7" s="126"/>
+      <c r="K7" s="127"/>
     </row>
     <row r="8" spans="1:20" outlineLevel="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="133"/>
-      <c r="C8" s="134"/>
-      <c r="D8" s="134"/>
-      <c r="E8" s="134"/>
-      <c r="F8" s="134"/>
-      <c r="G8" s="134"/>
-      <c r="H8" s="134"/>
-      <c r="I8" s="134"/>
-      <c r="J8" s="134"/>
-      <c r="K8" s="135"/>
+      <c r="B8" s="125"/>
+      <c r="C8" s="126"/>
+      <c r="D8" s="126"/>
+      <c r="E8" s="126"/>
+      <c r="F8" s="126"/>
+      <c r="G8" s="126"/>
+      <c r="H8" s="126"/>
+      <c r="I8" s="126"/>
+      <c r="J8" s="126"/>
+      <c r="K8" s="127"/>
     </row>
     <row r="9" spans="1:20" ht="31.5" customHeight="1" outlineLevel="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="136" t="s">
+      <c r="B9" s="128" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="137"/>
-      <c r="D9" s="137"/>
-      <c r="E9" s="137"/>
-      <c r="F9" s="137"/>
-      <c r="G9" s="137"/>
-      <c r="H9" s="137"/>
-      <c r="I9" s="137"/>
-      <c r="J9" s="137"/>
-      <c r="K9" s="138"/>
+      <c r="C9" s="129"/>
+      <c r="D9" s="129"/>
+      <c r="E9" s="129"/>
+      <c r="F9" s="129"/>
+      <c r="G9" s="129"/>
+      <c r="H9" s="129"/>
+      <c r="I9" s="129"/>
+      <c r="J9" s="129"/>
+      <c r="K9" s="130"/>
     </row>
     <row r="10" spans="1:20" ht="19.7" customHeight="1" outlineLevel="1" thickBot="1">
-      <c r="B10" s="139" t="s">
+      <c r="B10" s="131" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="140"/>
-      <c r="D10" s="140"/>
-      <c r="E10" s="140"/>
-      <c r="F10" s="140"/>
-      <c r="G10" s="140"/>
-      <c r="H10" s="140"/>
-      <c r="I10" s="140"/>
-      <c r="J10" s="140"/>
-      <c r="K10" s="141"/>
+      <c r="C10" s="132"/>
+      <c r="D10" s="132"/>
+      <c r="E10" s="132"/>
+      <c r="F10" s="132"/>
+      <c r="G10" s="132"/>
+      <c r="H10" s="132"/>
+      <c r="I10" s="132"/>
+      <c r="J10" s="132"/>
+      <c r="K10" s="133"/>
     </row>
     <row r="11" spans="1:20" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="A11" s="2"/>
@@ -2804,17 +2807,19 @@
         <v>#REF!</v>
       </c>
       <c r="L20" s="9"/>
-      <c r="M20" s="142" t="s">
+      <c r="M20" s="134" t="s">
         <v>38</v>
       </c>
-      <c r="N20" s="144" t="s">
+      <c r="N20" s="136" t="s">
         <v>36</v>
       </c>
-      <c r="O20" s="144" t="s">
+      <c r="O20" s="136" t="s">
         <v>37</v>
       </c>
-      <c r="P20" s="146"/>
-      <c r="Q20" s="142" t="s">
+      <c r="P20" s="138" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q20" s="134" t="s">
         <v>39</v>
       </c>
       <c r="T20" s="9"/>
@@ -2837,11 +2842,11 @@
         <v>#REF!</v>
       </c>
       <c r="L21" s="9"/>
-      <c r="M21" s="143"/>
-      <c r="N21" s="145"/>
-      <c r="O21" s="145"/>
-      <c r="P21" s="146"/>
-      <c r="Q21" s="142"/>
+      <c r="M21" s="135"/>
+      <c r="N21" s="137"/>
+      <c r="O21" s="137"/>
+      <c r="P21" s="138"/>
+      <c r="Q21" s="134"/>
       <c r="R21" s="11"/>
       <c r="T21" s="9"/>
     </row>
@@ -2905,12 +2910,12 @@
       <c r="K24" s="79"/>
       <c r="L24" s="9"/>
       <c r="M24" s="13"/>
-      <c r="N24" s="127" t="s">
+      <c r="N24" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="O24" s="128"/>
-      <c r="P24" s="128"/>
-      <c r="Q24" s="128"/>
+      <c r="O24" s="120"/>
+      <c r="P24" s="120"/>
+      <c r="Q24" s="120"/>
       <c r="R24" s="13"/>
       <c r="T24" s="9"/>
     </row>
@@ -3067,16 +3072,16 @@
       <c r="J30" s="70"/>
       <c r="K30" s="71"/>
       <c r="L30" s="9"/>
-      <c r="M30" s="116" t="s">
+      <c r="M30" s="139" t="s">
         <v>16</v>
       </c>
-      <c r="N30" s="118" t="s">
+      <c r="N30" s="141" t="s">
         <v>44</v>
       </c>
-      <c r="O30" s="120" t="s">
+      <c r="O30" s="143" t="s">
         <v>40</v>
       </c>
-      <c r="P30" s="122" t="s">
+      <c r="P30" s="145" t="s">
         <v>17</v>
       </c>
       <c r="T30" s="9"/>
@@ -3098,10 +3103,10 @@
       <c r="J31" s="70"/>
       <c r="K31" s="71"/>
       <c r="L31" s="9"/>
-      <c r="M31" s="117"/>
-      <c r="N31" s="119"/>
-      <c r="O31" s="121"/>
-      <c r="P31" s="123"/>
+      <c r="M31" s="140"/>
+      <c r="N31" s="142"/>
+      <c r="O31" s="144"/>
+      <c r="P31" s="146"/>
       <c r="T31" s="9"/>
     </row>
     <row r="32" spans="2:20" ht="15" customHeight="1" thickBot="1">
@@ -3162,10 +3167,10 @@
       <c r="N33" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="O33" s="120" t="s">
+      <c r="O33" s="143" t="s">
         <v>42</v>
       </c>
-      <c r="P33" s="122" t="s">
+      <c r="P33" s="145" t="s">
         <v>17</v>
       </c>
       <c r="T33" s="9"/>
@@ -3189,8 +3194,8 @@
       <c r="L34" s="9"/>
       <c r="M34" s="113"/>
       <c r="N34" s="115"/>
-      <c r="O34" s="121"/>
-      <c r="P34" s="123"/>
+      <c r="O34" s="144"/>
+      <c r="P34" s="146"/>
       <c r="Q34" s="9"/>
       <c r="R34" s="9"/>
       <c r="T34" s="9"/>
@@ -3266,7 +3271,7 @@
       </c>
       <c r="K37" s="87">
         <f ca="1">TODAY()</f>
-        <v>45918</v>
+        <v>45919</v>
       </c>
       <c r="L37" s="9"/>
       <c r="M37" s="73"/>
@@ -3283,16 +3288,16 @@
       <c r="K38" s="48"/>
     </row>
     <row r="39" spans="2:20" ht="19.5">
-      <c r="B39" s="124"/>
-      <c r="C39" s="125"/>
-      <c r="D39" s="125"/>
-      <c r="E39" s="125"/>
-      <c r="F39" s="125"/>
-      <c r="G39" s="125"/>
-      <c r="H39" s="125"/>
-      <c r="I39" s="125"/>
-      <c r="J39" s="125"/>
-      <c r="K39" s="126"/>
+      <c r="B39" s="116"/>
+      <c r="C39" s="117"/>
+      <c r="D39" s="117"/>
+      <c r="E39" s="117"/>
+      <c r="F39" s="117"/>
+      <c r="G39" s="117"/>
+      <c r="H39" s="117"/>
+      <c r="I39" s="117"/>
+      <c r="J39" s="117"/>
+      <c r="K39" s="118"/>
     </row>
     <row r="40" spans="2:20" ht="15" customHeight="1">
       <c r="B40" s="47"/>
@@ -3336,6 +3341,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="P33:P34"/>
     <mergeCell ref="B39:K39"/>
     <mergeCell ref="N24:Q24"/>
     <mergeCell ref="D3:G4"/>
@@ -3352,7 +3358,6 @@
     <mergeCell ref="O30:O31"/>
     <mergeCell ref="P30:P31"/>
     <mergeCell ref="O33:O34"/>
-    <mergeCell ref="P33:P34"/>
   </mergeCells>
   <phoneticPr fontId="34" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Adjust row positions for praca and doprava data in Excel export
Updated the starting row for praca and doprava data insertion to be dynamically based on last_item_row, improving placement logic in the Excel export process. Also added a minor formatting change at the end of the file.
</commit_message>
<xml_diff>
--- a/one folder to rule them all/Hlavna aplikacia/CPINT.xlsx
+++ b/one folder to rule them all/Hlavna aplikacia/CPINT.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="Tento_zošit"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slaso\Documents\GitHub\one folder to rule them all\Hlavna aplikacia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\LastMile\one folder to rule them all\Hlavna aplikacia\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD3A46C-5BBE-4B83-BB76-13755701FFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="5070" windowWidth="28800" windowHeight="15345"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CP" sheetId="30" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <definedName name="AND">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">CP!$B$2:$K$27</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -182,7 +183,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
     <numFmt numFmtId="164" formatCode="#,##0.00&quot; Sk&quot;"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ _S_k"/>
@@ -1426,7 +1427,7 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1588,7 +1589,6 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1706,6 +1706,12 @@
     <xf numFmtId="0" fontId="27" fillId="26" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="48" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="48" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1793,75 +1799,69 @@
     <xf numFmtId="0" fontId="48" fillId="21" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="61">
-    <cellStyle name="20 % - zvýraznenie1 2" xfId="16"/>
-    <cellStyle name="20 % - zvýraznenie2 2" xfId="17"/>
-    <cellStyle name="20 % - zvýraznenie3 2" xfId="18"/>
-    <cellStyle name="20 % - zvýraznenie4 2" xfId="19"/>
-    <cellStyle name="20 % - zvýraznenie5 2" xfId="20"/>
-    <cellStyle name="20 % - zvýraznenie6 2" xfId="21"/>
-    <cellStyle name="40 % - zvýraznenie1 2" xfId="22"/>
-    <cellStyle name="40 % - zvýraznenie2 2" xfId="23"/>
-    <cellStyle name="40 % - zvýraznenie3 2" xfId="24"/>
-    <cellStyle name="40 % - zvýraznenie4 2" xfId="25"/>
-    <cellStyle name="40 % - zvýraznenie5 2" xfId="26"/>
-    <cellStyle name="40 % - zvýraznenie6 2" xfId="27"/>
-    <cellStyle name="60 % - zvýraznenie1 2" xfId="28"/>
-    <cellStyle name="60 % - zvýraznenie2 2" xfId="29"/>
-    <cellStyle name="60 % - zvýraznenie3 2" xfId="30"/>
-    <cellStyle name="60 % - zvýraznenie4 2" xfId="31"/>
-    <cellStyle name="60 % - zvýraznenie5 2" xfId="32"/>
-    <cellStyle name="60 % - zvýraznenie6 2" xfId="33"/>
-    <cellStyle name="čiarky 2" xfId="7"/>
-    <cellStyle name="Dobrá 2" xfId="34"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8"/>
-    <cellStyle name="Hypertextové prepojenie 2" xfId="5"/>
-    <cellStyle name="Kontrolná bunka 2" xfId="35"/>
-    <cellStyle name="lehký dolní okraj" xfId="36"/>
-    <cellStyle name="Mena 2" xfId="37"/>
-    <cellStyle name="nadpis" xfId="38"/>
-    <cellStyle name="Nadpis 1 2" xfId="39"/>
-    <cellStyle name="Nadpis 2 2" xfId="40"/>
-    <cellStyle name="Nadpis 3 2" xfId="41"/>
-    <cellStyle name="Nadpis 4 2" xfId="42"/>
-    <cellStyle name="Neutrálna 2" xfId="43"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="8"/>
-    <cellStyle name="Normálna 2" xfId="2"/>
-    <cellStyle name="Normálna 2 2" xfId="14"/>
-    <cellStyle name="Normálna 3" xfId="15"/>
-    <cellStyle name="Normálna 4" xfId="60"/>
-    <cellStyle name="Normálna 6" xfId="12"/>
-    <cellStyle name="Normálna 7" xfId="13"/>
-    <cellStyle name="Normálne 2" xfId="1"/>
-    <cellStyle name="normálne 2 2" xfId="9"/>
-    <cellStyle name="Normálne 3" xfId="3"/>
-    <cellStyle name="Normálne 4" xfId="10"/>
-    <cellStyle name="Normálne 5" xfId="11"/>
-    <cellStyle name="normální 2" xfId="4"/>
-    <cellStyle name="normální_POL.XLS" xfId="6"/>
-    <cellStyle name="Poznámka 2" xfId="44"/>
-    <cellStyle name="Prepojená bunka 2" xfId="45"/>
-    <cellStyle name="Spolu 2" xfId="46"/>
-    <cellStyle name="Text upozornenia 2" xfId="47"/>
-    <cellStyle name="Vstup 2" xfId="48"/>
-    <cellStyle name="Výpočet 2" xfId="49"/>
-    <cellStyle name="Výstup 2" xfId="50"/>
-    <cellStyle name="Vysvetľujúci text 2" xfId="51"/>
-    <cellStyle name="Zlá 2" xfId="52"/>
-    <cellStyle name="Zvýraznenie1 2" xfId="53"/>
-    <cellStyle name="Zvýraznenie2 2" xfId="54"/>
-    <cellStyle name="Zvýraznenie3 2" xfId="55"/>
-    <cellStyle name="Zvýraznenie4 2" xfId="56"/>
-    <cellStyle name="Zvýraznenie5 2" xfId="57"/>
-    <cellStyle name="Zvýraznenie6 2" xfId="58"/>
+    <cellStyle name="20 % - zvýraznenie1 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="20 % - zvýraznenie2 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="20 % - zvýraznenie3 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="20 % - zvýraznenie4 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="20 % - zvýraznenie5 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="20 % - zvýraznenie6 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="40 % - zvýraznenie1 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="40 % - zvýraznenie2 2" xfId="23" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="40 % - zvýraznenie3 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="40 % - zvýraznenie4 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="40 % - zvýraznenie5 2" xfId="26" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="40 % - zvýraznenie6 2" xfId="27" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="60 % - zvýraznenie1 2" xfId="28" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="60 % - zvýraznenie2 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="60 % - zvýraznenie3 2" xfId="30" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="60 % - zvýraznenie4 2" xfId="31" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="60 % - zvýraznenie5 2" xfId="32" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="60 % - zvýraznenie6 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="čiarky 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Dobrá 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Hypertextové prepojenie" xfId="59" builtinId="8"/>
+    <cellStyle name="Hypertextové prepojenie 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Kontrolná bunka 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="lehký dolní okraj" xfId="36" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Mena 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="nadpis" xfId="38" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Nadpis 1 2" xfId="39" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Nadpis 2 2" xfId="40" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Nadpis 3 2" xfId="41" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Nadpis 4 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Neutrálna 2" xfId="43" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Normal 3" xfId="8" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
+    <cellStyle name="Normálna 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Normálna 2 2" xfId="14" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Normálna 3" xfId="15" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Normálna 4" xfId="60" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Normálna 6" xfId="12" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Normálna 7" xfId="13" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Normálne 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="normálne 2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Normálne 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Normálne 4" xfId="10" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Normálne 5" xfId="11" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="normální 2" xfId="4" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="normální_POL.XLS" xfId="6" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Poznámka 2" xfId="44" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Prepojená bunka 2" xfId="45" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Spolu 2" xfId="46" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Text upozornenia 2" xfId="47" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Vstup 2" xfId="48" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Výpočet 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Výstup 2" xfId="50" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Vysvetľujúci text 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Zlá 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="Zvýraznenie1 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="Zvýraznenie2 2" xfId="54" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="Zvýraznenie3 2" xfId="55" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Zvýraznenie4 2" xfId="56" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="Zvýraznenie5 2" xfId="57" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="Zvýraznenie6 2" xfId="58" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1910,7 +1910,7 @@
         <xdr:cNvPr id="14" name="Obrázok 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DB7B07B5-FAE2-FB54-2448-E1CCD3E523B6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB7B07B5-FAE2-FB54-2448-E1CCD3E523B6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1954,14 +1954,14 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>248</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>169677</xdr:rowOff>
+      <xdr:rowOff>12795</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="5" name="Obrázok 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{94490EEA-3500-4A23-96AC-19B01E18C0FE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94490EEA-3500-4A23-96AC-19B01E18C0FE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2010,7 +2010,7 @@
         <xdr:cNvPr id="4" name="Obrázok 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3F91FD3D-CBAA-C8DC-12EB-C06FEB5CD61F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F91FD3D-CBAA-C8DC-12EB-C06FEB5CD61F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2306,15 +2306,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hárok1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T57"/>
+  <dimension ref="A1:T37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="12" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M32" sqref="M32"/>
+      <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M22" sqref="M22:R37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2360,10 +2360,10 @@
       <c r="A3" s="1"/>
       <c r="B3" s="26"/>
       <c r="C3" s="27"/>
-      <c r="D3" s="116"/>
-      <c r="E3" s="116"/>
-      <c r="F3" s="116"/>
-      <c r="G3" s="116"/>
+      <c r="D3" s="117"/>
+      <c r="E3" s="117"/>
+      <c r="F3" s="117"/>
+      <c r="G3" s="117"/>
       <c r="H3" s="28"/>
       <c r="I3" s="28"/>
       <c r="J3" s="28"/>
@@ -2373,10 +2373,10 @@
       <c r="A4" s="1"/>
       <c r="B4" s="26"/>
       <c r="C4" s="27"/>
-      <c r="D4" s="116"/>
-      <c r="E4" s="116"/>
-      <c r="F4" s="116"/>
-      <c r="G4" s="116"/>
+      <c r="D4" s="117"/>
+      <c r="E4" s="117"/>
+      <c r="F4" s="117"/>
+      <c r="G4" s="117"/>
       <c r="H4" s="28"/>
       <c r="I4" s="28"/>
       <c r="J4" s="28"/>
@@ -2397,73 +2397,73 @@
     </row>
     <row r="6" spans="1:20" outlineLevel="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="117" t="s">
+      <c r="B6" s="118" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="118"/>
-      <c r="D6" s="118"/>
-      <c r="E6" s="118"/>
-      <c r="F6" s="118"/>
-      <c r="G6" s="118"/>
-      <c r="H6" s="118"/>
-      <c r="I6" s="118"/>
-      <c r="J6" s="118"/>
-      <c r="K6" s="119"/>
+      <c r="C6" s="119"/>
+      <c r="D6" s="119"/>
+      <c r="E6" s="119"/>
+      <c r="F6" s="119"/>
+      <c r="G6" s="119"/>
+      <c r="H6" s="119"/>
+      <c r="I6" s="119"/>
+      <c r="J6" s="119"/>
+      <c r="K6" s="120"/>
     </row>
     <row r="7" spans="1:20" outlineLevel="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="120"/>
-      <c r="C7" s="121"/>
-      <c r="D7" s="121"/>
-      <c r="E7" s="121"/>
-      <c r="F7" s="121"/>
-      <c r="G7" s="121"/>
-      <c r="H7" s="121"/>
-      <c r="I7" s="121"/>
-      <c r="J7" s="121"/>
-      <c r="K7" s="122"/>
+      <c r="B7" s="121"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="122"/>
+      <c r="G7" s="122"/>
+      <c r="H7" s="122"/>
+      <c r="I7" s="122"/>
+      <c r="J7" s="122"/>
+      <c r="K7" s="123"/>
     </row>
     <row r="8" spans="1:20" outlineLevel="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="120"/>
-      <c r="C8" s="121"/>
-      <c r="D8" s="121"/>
-      <c r="E8" s="121"/>
-      <c r="F8" s="121"/>
-      <c r="G8" s="121"/>
-      <c r="H8" s="121"/>
-      <c r="I8" s="121"/>
-      <c r="J8" s="121"/>
-      <c r="K8" s="122"/>
+      <c r="B8" s="121"/>
+      <c r="C8" s="122"/>
+      <c r="D8" s="122"/>
+      <c r="E8" s="122"/>
+      <c r="F8" s="122"/>
+      <c r="G8" s="122"/>
+      <c r="H8" s="122"/>
+      <c r="I8" s="122"/>
+      <c r="J8" s="122"/>
+      <c r="K8" s="123"/>
     </row>
     <row r="9" spans="1:20" ht="31.5" customHeight="1" outlineLevel="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="123" t="s">
+      <c r="B9" s="124" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="124"/>
-      <c r="D9" s="124"/>
-      <c r="E9" s="124"/>
-      <c r="F9" s="124"/>
-      <c r="G9" s="124"/>
-      <c r="H9" s="124"/>
-      <c r="I9" s="124"/>
-      <c r="J9" s="124"/>
-      <c r="K9" s="125"/>
+      <c r="C9" s="125"/>
+      <c r="D9" s="125"/>
+      <c r="E9" s="125"/>
+      <c r="F9" s="125"/>
+      <c r="G9" s="125"/>
+      <c r="H9" s="125"/>
+      <c r="I9" s="125"/>
+      <c r="J9" s="125"/>
+      <c r="K9" s="126"/>
     </row>
     <row r="10" spans="1:20" ht="19.7" customHeight="1" outlineLevel="1" thickBot="1">
-      <c r="B10" s="126" t="s">
+      <c r="B10" s="127" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="127"/>
-      <c r="D10" s="127"/>
-      <c r="E10" s="127"/>
-      <c r="F10" s="127"/>
-      <c r="G10" s="127"/>
-      <c r="H10" s="127"/>
-      <c r="I10" s="127"/>
-      <c r="J10" s="127"/>
-      <c r="K10" s="128"/>
+      <c r="C10" s="128"/>
+      <c r="D10" s="128"/>
+      <c r="E10" s="128"/>
+      <c r="F10" s="128"/>
+      <c r="G10" s="128"/>
+      <c r="H10" s="128"/>
+      <c r="I10" s="128"/>
+      <c r="J10" s="128"/>
+      <c r="K10" s="129"/>
     </row>
     <row r="11" spans="1:20" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="A11" s="2"/>
@@ -2511,25 +2511,25 @@
         <v>4</v>
       </c>
       <c r="L12" s="12"/>
-      <c r="M12" s="95" t="s">
+      <c r="M12" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="N12" s="95" t="s">
+      <c r="N12" s="94" t="s">
         <v>25</v>
       </c>
-      <c r="O12" s="95" t="s">
+      <c r="O12" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="P12" s="95" t="s">
+      <c r="P12" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="Q12" s="96" t="s">
+      <c r="Q12" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="R12" s="95" t="s">
+      <c r="R12" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="S12" s="96" t="s">
+      <c r="S12" s="95" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2556,16 +2556,16 @@
       <c r="T13" s="17"/>
     </row>
     <row r="14" spans="1:20" ht="20.25" customHeight="1">
-      <c r="B14" s="101"/>
-      <c r="C14" s="102"/>
-      <c r="D14" s="102"/>
-      <c r="E14" s="102"/>
-      <c r="F14" s="103"/>
-      <c r="G14" s="102"/>
-      <c r="H14" s="102"/>
-      <c r="I14" s="102"/>
-      <c r="J14" s="102"/>
-      <c r="K14" s="104"/>
+      <c r="B14" s="100"/>
+      <c r="C14" s="101"/>
+      <c r="D14" s="101"/>
+      <c r="E14" s="101"/>
+      <c r="F14" s="102"/>
+      <c r="G14" s="101"/>
+      <c r="H14" s="101"/>
+      <c r="I14" s="101"/>
+      <c r="J14" s="101"/>
+      <c r="K14" s="103"/>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
       <c r="N14" s="9"/>
@@ -2602,7 +2602,7 @@
         <f>#REF!+#REF!+#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="H16" s="70"/>
+      <c r="H16" s="69"/>
       <c r="I16" s="54" t="s">
         <v>37</v>
       </c>
@@ -2632,37 +2632,37 @@
       <c r="T17" s="9"/>
     </row>
     <row r="18" spans="2:20" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B18" s="88" t="s">
+      <c r="B18" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="89"/>
-      <c r="D18" s="90"/>
-      <c r="E18" s="90"/>
-      <c r="F18" s="90"/>
-      <c r="G18" s="90"/>
-      <c r="H18" s="90"/>
-      <c r="I18" s="90"/>
-      <c r="J18" s="91"/>
-      <c r="K18" s="71" t="s">
+      <c r="C18" s="88"/>
+      <c r="D18" s="89"/>
+      <c r="E18" s="89"/>
+      <c r="F18" s="89"/>
+      <c r="G18" s="89"/>
+      <c r="H18" s="89"/>
+      <c r="I18" s="89"/>
+      <c r="J18" s="90"/>
+      <c r="K18" s="70" t="s">
         <v>11</v>
       </c>
       <c r="L18" s="9"/>
       <c r="T18" s="9"/>
     </row>
     <row r="19" spans="2:20" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B19" s="84" t="e">
+      <c r="B19" s="83" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="C19" s="85"/>
-      <c r="D19" s="86"/>
-      <c r="E19" s="86"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="86"/>
-      <c r="H19" s="86"/>
-      <c r="I19" s="86"/>
-      <c r="J19" s="87"/>
-      <c r="K19" s="72" t="e">
+      <c r="C19" s="84"/>
+      <c r="D19" s="85"/>
+      <c r="E19" s="85"/>
+      <c r="F19" s="85"/>
+      <c r="G19" s="85"/>
+      <c r="H19" s="85"/>
+      <c r="I19" s="85"/>
+      <c r="J19" s="86"/>
+      <c r="K19" s="71" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
@@ -2670,19 +2670,19 @@
       <c r="T19" s="9"/>
     </row>
     <row r="20" spans="2:20" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B20" s="84" t="e">
+      <c r="B20" s="83" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="C20" s="85"/>
-      <c r="D20" s="86"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="86"/>
-      <c r="G20" s="86"/>
-      <c r="H20" s="86"/>
-      <c r="I20" s="86"/>
-      <c r="J20" s="87"/>
-      <c r="K20" s="72" t="e">
+      <c r="C20" s="84"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="85"/>
+      <c r="F20" s="85"/>
+      <c r="G20" s="85"/>
+      <c r="H20" s="85"/>
+      <c r="I20" s="85"/>
+      <c r="J20" s="86"/>
+      <c r="K20" s="71" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
@@ -2690,19 +2690,19 @@
       <c r="T20" s="9"/>
     </row>
     <row r="21" spans="2:20" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B21" s="84" t="e">
+      <c r="B21" s="83" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="C21" s="85"/>
-      <c r="D21" s="86"/>
-      <c r="E21" s="86"/>
-      <c r="F21" s="86"/>
-      <c r="G21" s="86"/>
-      <c r="H21" s="86"/>
-      <c r="I21" s="86"/>
-      <c r="J21" s="87"/>
-      <c r="K21" s="72" t="e">
+      <c r="C21" s="84"/>
+      <c r="D21" s="85"/>
+      <c r="E21" s="85"/>
+      <c r="F21" s="85"/>
+      <c r="G21" s="85"/>
+      <c r="H21" s="85"/>
+      <c r="I21" s="85"/>
+      <c r="J21" s="86"/>
+      <c r="K21" s="71" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
@@ -2718,7 +2718,7 @@
       <c r="G22" s="62"/>
       <c r="H22" s="62"/>
       <c r="I22" s="61"/>
-      <c r="J22" s="92" t="s">
+      <c r="J22" s="91" t="s">
         <v>41</v>
       </c>
       <c r="K22" s="64" t="e">
@@ -2726,6 +2726,21 @@
         <v>#REF!</v>
       </c>
       <c r="L22" s="9"/>
+      <c r="M22" s="130" t="s">
+        <v>29</v>
+      </c>
+      <c r="N22" s="132" t="s">
+        <v>27</v>
+      </c>
+      <c r="O22" s="132" t="s">
+        <v>28</v>
+      </c>
+      <c r="P22" s="134" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q22" s="130" t="s">
+        <v>30</v>
+      </c>
       <c r="T22" s="9"/>
     </row>
     <row r="23" spans="2:20" ht="18.75" thickBot="1">
@@ -2740,22 +2755,34 @@
       <c r="J23" s="66"/>
       <c r="K23" s="67"/>
       <c r="L23" s="9"/>
+      <c r="M23" s="131"/>
+      <c r="N23" s="133"/>
+      <c r="O23" s="133"/>
+      <c r="P23" s="134"/>
+      <c r="Q23" s="130"/>
+      <c r="R23" s="11"/>
       <c r="T23" s="9"/>
     </row>
     <row r="24" spans="2:20" ht="20.100000000000001" customHeight="1">
-      <c r="B24" s="73" t="s">
+      <c r="B24" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="74"/>
-      <c r="D24" s="74"/>
-      <c r="E24" s="74"/>
-      <c r="F24" s="74"/>
-      <c r="G24" s="74"/>
-      <c r="H24" s="74"/>
-      <c r="I24" s="74"/>
-      <c r="J24" s="74"/>
-      <c r="K24" s="75"/>
+      <c r="C24" s="73"/>
+      <c r="D24" s="73"/>
+      <c r="E24" s="73"/>
+      <c r="F24" s="73"/>
+      <c r="G24" s="73"/>
+      <c r="H24" s="73"/>
+      <c r="I24" s="73"/>
+      <c r="J24" s="73"/>
+      <c r="K24" s="74"/>
       <c r="L24" s="9"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="12"/>
       <c r="T24" s="9"/>
     </row>
     <row r="25" spans="2:20" ht="15.75" thickBot="1">
@@ -2770,104 +2797,196 @@
       <c r="J25" s="18"/>
       <c r="K25" s="68"/>
       <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
       <c r="T25" s="9"/>
     </row>
     <row r="26" spans="2:20" ht="20.100000000000001" customHeight="1">
-      <c r="B26" s="76" t="s">
+      <c r="B26" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="77"/>
-      <c r="F26" s="77"/>
-      <c r="G26" s="77"/>
-      <c r="H26" s="77"/>
-      <c r="I26" s="77"/>
-      <c r="J26" s="77"/>
-      <c r="K26" s="78"/>
+      <c r="C26" s="76"/>
+      <c r="D26" s="76"/>
+      <c r="E26" s="76"/>
+      <c r="F26" s="76"/>
+      <c r="G26" s="76"/>
+      <c r="H26" s="76"/>
+      <c r="I26" s="76"/>
+      <c r="J26" s="76"/>
+      <c r="K26" s="77"/>
       <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9"/>
-      <c r="Q26" s="9"/>
-      <c r="R26" s="9"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="115" t="s">
+        <v>12</v>
+      </c>
+      <c r="O26" s="116"/>
+      <c r="P26" s="116"/>
+      <c r="Q26" s="116"/>
+      <c r="R26" s="13"/>
       <c r="S26" s="9"/>
       <c r="T26" s="9"/>
     </row>
     <row r="27" spans="2:20" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B27" s="79"/>
-      <c r="C27" s="80" t="s">
+      <c r="B27" s="78"/>
+      <c r="C27" s="79" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="81"/>
-      <c r="E27" s="81"/>
-      <c r="F27" s="81"/>
-      <c r="G27" s="81"/>
-      <c r="H27" s="81"/>
-      <c r="I27" s="81"/>
-      <c r="J27" s="82" t="s">
+      <c r="D27" s="80"/>
+      <c r="E27" s="80"/>
+      <c r="F27" s="80"/>
+      <c r="G27" s="80"/>
+      <c r="H27" s="80"/>
+      <c r="I27" s="80"/>
+      <c r="J27" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="K27" s="83">
+      <c r="K27" s="82">
         <f ca="1">TODAY()</f>
-        <v>45921</v>
+        <v>45925</v>
       </c>
       <c r="L27" s="9"/>
-      <c r="M27" s="69"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="9"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O27" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="P27" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q27" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="R27" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="S27" s="9"/>
       <c r="T27" s="9"/>
     </row>
     <row r="28" spans="2:20">
       <c r="B28" s="47"/>
       <c r="K28" s="48"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="96"/>
+      <c r="O28" s="97"/>
+      <c r="P28" s="98"/>
+      <c r="Q28" s="98"/>
+      <c r="R28" s="8"/>
     </row>
     <row r="29" spans="2:20" ht="19.5">
-      <c r="B29" s="111"/>
-      <c r="C29" s="112"/>
-      <c r="D29" s="112"/>
-      <c r="E29" s="112"/>
-      <c r="F29" s="112"/>
-      <c r="G29" s="112"/>
-      <c r="H29" s="112"/>
-      <c r="I29" s="112"/>
-      <c r="J29" s="112"/>
-      <c r="K29" s="113"/>
+      <c r="B29" s="112"/>
+      <c r="C29" s="113"/>
+      <c r="D29" s="113"/>
+      <c r="E29" s="113"/>
+      <c r="F29" s="113"/>
+      <c r="G29" s="113"/>
+      <c r="H29" s="113"/>
+      <c r="I29" s="113"/>
+      <c r="J29" s="113"/>
+      <c r="K29" s="114"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="96"/>
+      <c r="O29" s="97"/>
+      <c r="P29" s="98"/>
+      <c r="Q29" s="98"/>
+      <c r="R29" s="8"/>
     </row>
     <row r="30" spans="2:20" ht="15" customHeight="1">
       <c r="B30" s="47"/>
       <c r="K30" s="48"/>
-    </row>
-    <row r="31" spans="2:20">
+      <c r="M30" s="5"/>
+      <c r="N30" s="96"/>
+      <c r="O30" s="97"/>
+      <c r="P30" s="98"/>
+      <c r="Q30" s="98"/>
+      <c r="R30" s="8"/>
+    </row>
+    <row r="31" spans="2:20" ht="15.75" thickBot="1">
       <c r="B31" s="47"/>
       <c r="K31" s="48"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="96"/>
+      <c r="O31" s="97"/>
+      <c r="P31" s="98"/>
+      <c r="Q31" s="98"/>
+      <c r="R31" s="8"/>
     </row>
     <row r="32" spans="2:20">
       <c r="B32" s="47"/>
       <c r="K32" s="48"/>
+      <c r="M32" s="135" t="s">
+        <v>16</v>
+      </c>
+      <c r="N32" s="137" t="s">
+        <v>35</v>
+      </c>
+      <c r="O32" s="108" t="s">
+        <v>31</v>
+      </c>
+      <c r="P32" s="110" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="33" spans="2:18" ht="15" customHeight="1">
       <c r="B33" s="47"/>
       <c r="K33" s="48"/>
-    </row>
-    <row r="34" spans="2:18" ht="15" customHeight="1">
+      <c r="M33" s="136"/>
+      <c r="N33" s="138"/>
+      <c r="O33" s="109"/>
+      <c r="P33" s="111"/>
+    </row>
+    <row r="34" spans="2:18" ht="15" customHeight="1" thickBot="1">
       <c r="B34" s="47"/>
       <c r="K34" s="48"/>
-    </row>
-    <row r="35" spans="2:18">
+      <c r="M34" s="99" t="e">
+        <f>SUM(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="N34" s="99" t="e">
+        <f>G16</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O34" s="14" t="e">
+        <f>N34-M34</f>
+        <v>#REF!</v>
+      </c>
+      <c r="P34" s="15" t="e">
+        <f>O34/N34</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="35" spans="2:18" ht="26.25">
       <c r="B35" s="47"/>
       <c r="K35" s="48"/>
+      <c r="M35" s="104" t="s">
+        <v>18</v>
+      </c>
+      <c r="N35" s="106" t="s">
+        <v>19</v>
+      </c>
+      <c r="O35" s="108" t="s">
+        <v>33</v>
+      </c>
+      <c r="P35" s="110" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="36" spans="2:18">
       <c r="B36" s="47"/>
       <c r="K36" s="48"/>
-    </row>
-    <row r="37" spans="2:18" ht="15.75" thickBot="1">
+      <c r="M36" s="105"/>
+      <c r="N36" s="107"/>
+      <c r="O36" s="109"/>
+      <c r="P36" s="111"/>
+      <c r="Q36" s="9"/>
+      <c r="R36" s="9"/>
+    </row>
+    <row r="37" spans="2:18" ht="16.5" thickBot="1">
       <c r="B37" s="49"/>
       <c r="C37" s="50"/>
       <c r="D37" s="50"/>
@@ -2878,207 +2997,44 @@
       <c r="I37" s="50"/>
       <c r="J37" s="50"/>
       <c r="K37" s="51"/>
-    </row>
-    <row r="42" spans="2:18">
-      <c r="M42" s="129" t="s">
-        <v>29</v>
-      </c>
-      <c r="N42" s="131" t="s">
-        <v>27</v>
-      </c>
-      <c r="O42" s="131" t="s">
-        <v>28</v>
-      </c>
-      <c r="P42" s="133" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q42" s="129" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="43" spans="2:18">
-      <c r="M43" s="130"/>
-      <c r="N43" s="132"/>
-      <c r="O43" s="132"/>
-      <c r="P43" s="133"/>
-      <c r="Q43" s="129"/>
-      <c r="R43" s="11"/>
-    </row>
-    <row r="44" spans="2:18">
-      <c r="M44" s="10"/>
-      <c r="N44" s="10"/>
-      <c r="O44" s="10"/>
-      <c r="P44" s="9"/>
-      <c r="Q44" s="12"/>
-      <c r="R44" s="12"/>
-    </row>
-    <row r="45" spans="2:18">
-      <c r="M45" s="9"/>
-      <c r="N45" s="9"/>
-      <c r="O45" s="9"/>
-      <c r="P45" s="9"/>
-      <c r="Q45" s="9"/>
-      <c r="R45" s="9"/>
-    </row>
-    <row r="46" spans="2:18">
-      <c r="M46" s="13"/>
-      <c r="N46" s="114" t="s">
-        <v>12</v>
-      </c>
-      <c r="O46" s="115"/>
-      <c r="P46" s="115"/>
-      <c r="Q46" s="115"/>
-      <c r="R46" s="13"/>
-    </row>
-    <row r="47" spans="2:18">
-      <c r="M47" s="13"/>
-      <c r="N47" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="O47" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="P47" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q47" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="R47" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="48" spans="2:18">
-      <c r="M48" s="5"/>
-      <c r="N48" s="97"/>
-      <c r="O48" s="98"/>
-      <c r="P48" s="99"/>
-      <c r="Q48" s="99"/>
-      <c r="R48" s="8"/>
-    </row>
-    <row r="49" spans="13:18">
-      <c r="M49" s="5"/>
-      <c r="N49" s="97"/>
-      <c r="O49" s="98"/>
-      <c r="P49" s="99"/>
-      <c r="Q49" s="99"/>
-      <c r="R49" s="8"/>
-    </row>
-    <row r="50" spans="13:18">
-      <c r="M50" s="5"/>
-      <c r="N50" s="97"/>
-      <c r="O50" s="98"/>
-      <c r="P50" s="99"/>
-      <c r="Q50" s="99"/>
-      <c r="R50" s="8"/>
-    </row>
-    <row r="51" spans="13:18" ht="15.75" thickBot="1">
-      <c r="M51" s="5"/>
-      <c r="N51" s="97"/>
-      <c r="O51" s="98"/>
-      <c r="P51" s="99"/>
-      <c r="Q51" s="99"/>
-      <c r="R51" s="8"/>
-    </row>
-    <row r="52" spans="13:18">
-      <c r="M52" s="134" t="s">
-        <v>16</v>
-      </c>
-      <c r="N52" s="136" t="s">
-        <v>35</v>
-      </c>
-      <c r="O52" s="138" t="s">
-        <v>31</v>
-      </c>
-      <c r="P52" s="109" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="53" spans="13:18">
-      <c r="M53" s="135"/>
-      <c r="N53" s="137"/>
-      <c r="O53" s="139"/>
-      <c r="P53" s="110"/>
-    </row>
-    <row r="54" spans="13:18" ht="16.5" thickBot="1">
-      <c r="M54" s="100" t="e">
-        <f>SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N54" s="100" t="e">
-        <f>G16</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O54" s="14" t="e">
-        <f>N54-M54</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P54" s="15" t="e">
-        <f>O54/N54</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="55" spans="13:18" ht="26.25">
-      <c r="M55" s="105" t="s">
-        <v>18</v>
-      </c>
-      <c r="N55" s="107" t="s">
-        <v>19</v>
-      </c>
-      <c r="O55" s="138" t="s">
-        <v>33</v>
-      </c>
-      <c r="P55" s="109" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="56" spans="13:18">
-      <c r="M56" s="106"/>
-      <c r="N56" s="108"/>
-      <c r="O56" s="139"/>
-      <c r="P56" s="110"/>
-      <c r="Q56" s="9"/>
-      <c r="R56" s="9"/>
-    </row>
-    <row r="57" spans="13:18" ht="16.5" thickBot="1">
-      <c r="M57" s="93">
-        <f>Q48+Q49+Q50+Q51</f>
+      <c r="M37" s="92">
+        <f>Q28+Q29+Q30+Q31</f>
         <v>0</v>
       </c>
-      <c r="N57" s="94" t="e">
+      <c r="N37" s="93" t="e">
         <f>J16</f>
         <v>#REF!</v>
       </c>
-      <c r="O57" s="14" t="e">
-        <f>N57-M57</f>
+      <c r="O37" s="14" t="e">
+        <f>N37-M37</f>
         <v>#REF!</v>
       </c>
-      <c r="P57" s="15" t="e">
-        <f>O57/N57</f>
+      <c r="P37" s="15" t="e">
+        <f>O37/N37</f>
         <v>#REF!</v>
       </c>
-      <c r="Q57" s="9"/>
-      <c r="R57" s="9"/>
+      <c r="Q37" s="9"/>
+      <c r="R37" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="O55:O56"/>
-    <mergeCell ref="P55:P56"/>
+    <mergeCell ref="P32:P33"/>
+    <mergeCell ref="O35:O36"/>
+    <mergeCell ref="P35:P36"/>
     <mergeCell ref="B29:K29"/>
-    <mergeCell ref="N46:Q46"/>
+    <mergeCell ref="N26:Q26"/>
     <mergeCell ref="D3:G4"/>
     <mergeCell ref="B6:K8"/>
     <mergeCell ref="B9:K9"/>
     <mergeCell ref="B10:K10"/>
-    <mergeCell ref="M42:M43"/>
-    <mergeCell ref="N42:N43"/>
-    <mergeCell ref="O42:O43"/>
-    <mergeCell ref="Q42:Q43"/>
-    <mergeCell ref="P42:P43"/>
-    <mergeCell ref="M52:M53"/>
-    <mergeCell ref="N52:N53"/>
-    <mergeCell ref="O52:O53"/>
-    <mergeCell ref="P52:P53"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="Q22:Q23"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="M32:M33"/>
+    <mergeCell ref="N32:N33"/>
+    <mergeCell ref="O32:O33"/>
   </mergeCells>
   <phoneticPr fontId="34" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>